<commit_message>
Update UKRIN config file
</commit_message>
<xml_diff>
--- a/config/ukrin_conf.xlsx
+++ b/config/ukrin_conf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\martin\code\xnat-dicomqc\docker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\martin\code\xnat-dicomqc\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2737A6C-3C71-48C8-98CB-10D0D695D461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B141FAD-83E2-48C1-98AB-B31FF163F4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1410" windowWidth="24795" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series names" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="293">
   <si>
     <t>Vendors</t>
   </si>
@@ -716,9 +716,6 @@
     <t>MTR_ON</t>
   </si>
   <si>
-    <t>T1MAP,T1MAP_FLIPPED,T2STAR,DWI,BASE,FAIR,PCASL,MTR</t>
-  </si>
-  <si>
     <t>Note all PCASL are not 'B0map PCASL'</t>
   </si>
   <si>
@@ -734,21 +731,12 @@
     <t>T1map,T1MAP_FLIPPED,BASE,FAIR,PCASL,DWI, DWI_FLIPPED</t>
   </si>
   <si>
-    <t>T1MAP,T1MAP_FLIPPED,T2_MAPPING,BASE,FAIR,PCASL,MDIXON,B0</t>
-  </si>
-  <si>
     <t>T1MAP,T1MAP_FLIPPED,T2_MAPPING,T2STAR,DWI,BASE,FAIR,PCASL,MDIXON</t>
   </si>
   <si>
     <t>T1MAP,T1MAP_FLIPPED,T2_MAPPING,T2STAR,BASE,FAIR,PCASL,MTR,MDIXON</t>
   </si>
   <si>
-    <t>T1MAP,T2_MAPPING,DWI,ASL,BASE,FAIR,PCASL,MDIXON</t>
-  </si>
-  <si>
-    <t>T1MAP,T1MAP_FLIPPED,T2STAR,BASE,FAIR,PCASL,MTR,MDIXON</t>
-  </si>
-  <si>
     <t>T1MAP,T1MAP_FLIPPED,T2_MAPPING,T2STAR,DWI,BASE,FAIR,PCASL,MTR,MDIXON</t>
   </si>
   <si>
@@ -899,14 +887,41 @@
     <t>[45, 65]</t>
   </si>
   <si>
-    <t>[3,9]</t>
+    <t>T1MAP,T1MAP_FLIPPED,T2_MAPPING,T2STAR,BASE,FAIR,PCASL</t>
+  </si>
+  <si>
+    <t>DWI,DWI_FLIPPED,B1MAP</t>
+  </si>
+  <si>
+    <t>T1MAP,T1MAP_FLIPPED,T2STAR,BASE,FAIR,PCASL,MTR</t>
+  </si>
+  <si>
+    <t>T1MAP,T1MAP_FLIPPED,T2STAR,BASE,FAIR,PCASL,MTR,NDIXON</t>
+  </si>
+  <si>
+    <t>T1MAP,T1MAP_FLIPPED,T2_MAPPING,BASE,FAIR,PCASL,B0</t>
+  </si>
+  <si>
+    <t>WARNING IF FAIL</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>T1MAP,T2_MAPPING,DWI,ASL,BASE,FAIR,PCASL</t>
+  </si>
+  <si>
+    <t>T1MAP,T1MAP_FLIPPED,T2STAR,DWI,BASE,FAIR,PCASL</t>
+  </si>
+  <si>
+    <t>[3, 9]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,6 +947,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1060,7 +1083,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1231,6 +1254,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1528,16 +1574,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>207</v>
@@ -1545,7 +1591,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1554,7 +1600,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1575,7 +1621,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1592,12 +1638,12 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C8" t="s">
         <v>51</v>
@@ -1627,10 +1673,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1641,7 +1687,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1674,7 +1720,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -1710,7 +1756,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1809,7 +1855,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="82" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -1820,7 +1866,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="82" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -1831,7 +1877,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="82" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1842,7 +1888,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="82" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -1853,7 +1899,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="83" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -1886,7 +1932,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="83" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -1897,7 +1943,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="83" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -1908,7 +1954,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="83" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -1930,7 +1976,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
@@ -1944,7 +1990,7 @@
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
@@ -2002,7 +2048,7 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C44" t="s">
         <v>33</v>
@@ -2273,7 +2319,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C71" t="s">
         <v>51</v>
@@ -2295,7 +2341,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C73" t="s">
         <v>51</v>
@@ -2306,7 +2352,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C74" t="s">
         <v>51</v>
@@ -2394,7 +2440,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C82" t="s">
         <v>51</v>
@@ -2466,11 +2512,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:L123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H104" sqref="H104"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,11 +2530,12 @@
     <col min="7" max="7" width="15.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" style="5" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="33" style="60" customWidth="1"/>
+    <col min="11" max="11" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>198</v>
       </c>
@@ -2516,13 +2563,16 @@
       <c r="I1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="93" t="s">
+        <v>288</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B2" s="72"/>
       <c r="C2" t="s">
@@ -2541,9 +2591,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
-        <v>232</v>
+        <v>287</v>
       </c>
       <c r="B3" s="91" t="s">
         <v>222</v>
@@ -2564,9 +2614,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
-        <v>226</v>
+        <v>291</v>
       </c>
       <c r="B4" s="91" t="s">
         <v>222</v>
@@ -2587,12 +2637,13 @@
         <v>5</v>
       </c>
       <c r="K4" s="60" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="L4" s="60"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" t="s">
@@ -2611,9 +2662,9 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" t="s">
@@ -2631,13 +2682,14 @@
       <c r="H6" s="5">
         <v>5</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="83" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="59"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" t="s">
@@ -2656,9 +2708,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B8" s="91" t="s">
         <v>222</v>
@@ -2676,9 +2728,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>235</v>
+        <v>290</v>
       </c>
       <c r="B9" s="72"/>
       <c r="E9" s="2" t="s">
@@ -2694,7 +2746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>204</v>
       </c>
@@ -2712,9 +2764,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B11" s="72"/>
       <c r="E11" s="2" t="s">
@@ -2733,7 +2785,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
         <v>9</v>
       </c>
@@ -2754,7 +2806,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>9</v>
       </c>
@@ -2773,15 +2825,18 @@
         <v>79</v>
       </c>
       <c r="H13" s="81" t="s">
-        <v>281</v>
+        <v>277</v>
+      </c>
+      <c r="J13" s="60" t="s">
+        <v>289</v>
       </c>
       <c r="K13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
-        <v>236</v>
+        <v>286</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" t="s">
@@ -2802,17 +2857,18 @@
       <c r="K14" s="34" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="34"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
-        <v>236</v>
+        <v>285</v>
       </c>
       <c r="B15" s="72"/>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F15" t="s">
         <v>102</v>
@@ -2821,13 +2877,14 @@
         <v>79</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="34"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" t="s">
@@ -2848,10 +2905,11 @@
       <c r="K16" s="34" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="34"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" t="s">
@@ -2870,13 +2928,14 @@
         <v>111</v>
       </c>
       <c r="K17" s="34"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="34"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B18" s="72"/>
-      <c r="C18" t="s">
+      <c r="C18" s="92" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="10" t="s">
@@ -2892,12 +2951,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B19" s="72"/>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="92" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -2913,12 +2972,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B20" s="72"/>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="92" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -2934,16 +2993,16 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B21" s="72"/>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="92" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F21" t="s">
         <v>117</v>
@@ -2955,16 +3014,16 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B22" s="72"/>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="92" t="s">
         <v>51</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F22" t="s">
         <v>117</v>
@@ -2976,7 +3035,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
         <v>118</v>
       </c>
@@ -2998,8 +3057,9 @@
         <v>121</v>
       </c>
       <c r="I23" s="69"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="94"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>203</v>
       </c>
@@ -3021,8 +3081,9 @@
         <v>12</v>
       </c>
       <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="95"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>203</v>
       </c>
@@ -3044,14 +3105,15 @@
         <v>12</v>
       </c>
       <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="95"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>203</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="6" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="11" t="s">
@@ -3067,8 +3129,9 @@
         <v>129</v>
       </c>
       <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="95"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>203</v>
       </c>
@@ -3087,11 +3150,12 @@
         <v>128</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="95"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>203</v>
       </c>
@@ -3111,8 +3175,9 @@
         <v>132</v>
       </c>
       <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="95"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>203</v>
       </c>
@@ -3132,8 +3197,9 @@
         <v>80</v>
       </c>
       <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="95"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>203</v>
       </c>
@@ -3155,8 +3221,9 @@
       <c r="I30" s="6">
         <v>299.60000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="95"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>23</v>
       </c>
@@ -3178,8 +3245,9 @@
         <v>4.5</v>
       </c>
       <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="96"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>23</v>
       </c>
@@ -3201,8 +3269,9 @@
         <v>10</v>
       </c>
       <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="96"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>23</v>
       </c>
@@ -3224,8 +3293,9 @@
         <v>10</v>
       </c>
       <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="96"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>23</v>
       </c>
@@ -3245,14 +3315,15 @@
         <v>139</v>
       </c>
       <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="96"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="15" t="s">
@@ -3268,8 +3339,9 @@
         <v>140</v>
       </c>
       <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="96"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>23</v>
       </c>
@@ -3291,8 +3363,9 @@
         <v>141</v>
       </c>
       <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="96"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>23</v>
       </c>
@@ -3314,8 +3387,9 @@
       <c r="I37" s="12">
         <v>299.60000000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="96"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>23</v>
       </c>
@@ -3337,8 +3411,9 @@
         <v>143</v>
       </c>
       <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="96"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>23</v>
       </c>
@@ -3360,8 +3435,9 @@
         <v>144</v>
       </c>
       <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="96"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>23</v>
       </c>
@@ -3371,7 +3447,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>102</v>
@@ -3380,11 +3456,12 @@
         <v>79</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="96"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>23</v>
       </c>
@@ -3406,8 +3483,9 @@
         <v>145</v>
       </c>
       <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="96"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>23</v>
       </c>
@@ -3429,8 +3507,9 @@
         <v>5</v>
       </c>
       <c r="I42" s="12"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="96"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="61" t="s">
         <v>19</v>
       </c>
@@ -3450,8 +3529,9 @@
         <v>147</v>
       </c>
       <c r="I43" s="18"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="97"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="61" t="s">
         <v>19</v>
       </c>
@@ -3471,8 +3551,9 @@
         <v>155</v>
       </c>
       <c r="I44" s="18"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="97"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="61" t="s">
         <v>19</v>
       </c>
@@ -3494,8 +3575,9 @@
       <c r="I45" s="18">
         <v>787.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="97"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="61" t="s">
         <v>19</v>
       </c>
@@ -3515,8 +3597,9 @@
         <v>110</v>
       </c>
       <c r="I46" s="18"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="97"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="61" t="s">
         <v>19</v>
       </c>
@@ -3538,8 +3621,9 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I47" s="18"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="97"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="61" t="s">
         <v>19</v>
       </c>
@@ -3561,8 +3645,9 @@
         <v>2.46</v>
       </c>
       <c r="I48" s="18"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J48" s="97"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="61" t="s">
         <v>19</v>
       </c>
@@ -3584,8 +3669,9 @@
         <v>17</v>
       </c>
       <c r="I49" s="18"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J49" s="97"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="61" t="s">
         <v>19</v>
       </c>
@@ -3607,8 +3693,9 @@
         <v>17</v>
       </c>
       <c r="I50" s="18"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J50" s="97"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="61" t="s">
         <v>19</v>
       </c>
@@ -3630,11 +3717,13 @@
         <v>152</v>
       </c>
       <c r="I51" s="18"/>
+      <c r="J51" s="97"/>
       <c r="K51" s="34" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="34"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="61" t="s">
         <v>19</v>
       </c>
@@ -3656,8 +3745,9 @@
         <v>154</v>
       </c>
       <c r="I52" s="18"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J52" s="97"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="62" t="s">
         <v>21</v>
       </c>
@@ -3679,8 +3769,9 @@
         <v>140</v>
       </c>
       <c r="I53" s="22"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J53" s="98"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="62" t="s">
         <v>21</v>
       </c>
@@ -3702,8 +3793,9 @@
       <c r="I54" s="22">
         <v>877</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J54" s="98"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="62" t="s">
         <v>21</v>
       </c>
@@ -3725,8 +3817,9 @@
       <c r="I55" s="22">
         <v>787.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J55" s="98"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="62" t="s">
         <v>21</v>
       </c>
@@ -3748,8 +3841,9 @@
       <c r="I56" s="22">
         <v>61</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J56" s="98"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="62" t="s">
         <v>21</v>
       </c>
@@ -3771,8 +3865,9 @@
         <v>60</v>
       </c>
       <c r="I57" s="22"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J57" s="98"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="62" t="s">
         <v>21</v>
       </c>
@@ -3796,8 +3891,9 @@
       <c r="I58" s="22">
         <v>62</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J58" s="98"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="62" t="s">
         <v>21</v>
       </c>
@@ -3819,8 +3915,9 @@
         <v>17</v>
       </c>
       <c r="I59" s="22"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J59" s="98"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="62" t="s">
         <v>21</v>
       </c>
@@ -3842,8 +3939,9 @@
         <v>17</v>
       </c>
       <c r="I60" s="22"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J60" s="98"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="62" t="s">
         <v>21</v>
       </c>
@@ -3865,11 +3963,13 @@
         <v>152</v>
       </c>
       <c r="I61" s="22"/>
+      <c r="J61" s="98"/>
       <c r="K61" s="34" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="34"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="62" t="s">
         <v>21</v>
       </c>
@@ -3891,10 +3991,11 @@
         <v>145</v>
       </c>
       <c r="I62" s="22"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J62" s="98"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B63" s="58"/>
       <c r="C63" s="26"/>
@@ -3912,10 +4013,11 @@
         <v>140</v>
       </c>
       <c r="I63" s="26"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J63" s="99"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B64" s="58"/>
       <c r="C64" s="27" t="s">
@@ -3937,10 +4039,11 @@
       <c r="I64" s="27">
         <v>3000</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J64" s="100"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B65" s="58"/>
       <c r="C65" s="27"/>
@@ -3960,10 +4063,11 @@
       <c r="I65" s="27">
         <v>1988</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J65" s="100"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B66" s="58"/>
       <c r="C66" s="27"/>
@@ -3978,15 +4082,16 @@
         <v>137</v>
       </c>
       <c r="H66" s="27" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I66" s="27">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J66" s="100"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="58" t="s">
-        <v>230</v>
+        <v>284</v>
       </c>
       <c r="B67" s="58"/>
       <c r="C67" s="27" t="s">
@@ -4006,10 +4111,11 @@
         <v>13</v>
       </c>
       <c r="I67" s="27"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J67" s="100"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B68" s="58"/>
       <c r="C68" s="27" t="s">
@@ -4029,8 +4135,9 @@
         <v>13</v>
       </c>
       <c r="I68" s="27"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J68" s="100"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
         <v>5</v>
       </c>
@@ -4054,8 +4161,9 @@
         <v>2</v>
       </c>
       <c r="I69" s="30"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J69" s="101"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
         <v>5</v>
       </c>
@@ -4079,8 +4187,9 @@
         <v>158</v>
       </c>
       <c r="I70" s="30"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J70" s="101"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>5</v>
       </c>
@@ -4101,11 +4210,12 @@
         <v>128</v>
       </c>
       <c r="H71" s="81" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I71" s="30"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J71" s="101"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
         <v>5</v>
       </c>
@@ -4124,11 +4234,12 @@
         <v>185</v>
       </c>
       <c r="H72" s="78" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="I72" s="30"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J72" s="101"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="80" t="s">
         <v>5</v>
       </c>
@@ -4150,11 +4261,12 @@
         <v>205</v>
       </c>
       <c r="I73" s="59"/>
-      <c r="J73" t="s">
+      <c r="J73" s="102"/>
+      <c r="K73" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
         <v>5</v>
       </c>
@@ -4178,8 +4290,9 @@
       <c r="I74" s="30">
         <v>787.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J74" s="101"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="63" t="s">
         <v>9</v>
       </c>
@@ -4201,8 +4314,9 @@
       <c r="I75" s="34">
         <v>1.68</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J75" s="103"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="63" t="s">
         <v>9</v>
       </c>
@@ -4222,8 +4336,9 @@
         <v>160</v>
       </c>
       <c r="I76" s="34"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J76" s="103"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="63" t="s">
         <v>9</v>
       </c>
@@ -4245,8 +4360,9 @@
       <c r="I77" s="34">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J77" s="103"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="63" t="s">
         <v>9</v>
       </c>
@@ -4268,8 +4384,9 @@
       <c r="I78" s="34">
         <v>787.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J78" s="103"/>
+    </row>
+    <row r="79" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="63" t="s">
         <v>9</v>
       </c>
@@ -4287,8 +4404,9 @@
       <c r="G79" s="36"/>
       <c r="H79" s="35"/>
       <c r="I79" s="34"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J79" s="103"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="63" t="s">
         <v>9</v>
       </c>
@@ -4308,8 +4426,9 @@
         <v>60</v>
       </c>
       <c r="I80" s="34"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="103"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="63" t="s">
         <v>9</v>
       </c>
@@ -4331,8 +4450,9 @@
         <v>1000</v>
       </c>
       <c r="I81" s="34"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" s="103"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="63" t="s">
         <v>9</v>
       </c>
@@ -4352,8 +4472,9 @@
         <v>202</v>
       </c>
       <c r="I82" s="34"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" s="103"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="63" t="s">
         <v>9</v>
       </c>
@@ -4373,8 +4494,9 @@
         <v>8</v>
       </c>
       <c r="I83" s="34"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" s="103"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="64" t="s">
         <v>210</v>
       </c>
@@ -4396,8 +4518,9 @@
       <c r="I84" s="38">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" s="104"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="64" t="s">
         <v>210</v>
       </c>
@@ -4417,14 +4540,15 @@
         <v>160</v>
       </c>
       <c r="I85" s="38"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" s="104"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="s">
         <v>210</v>
       </c>
       <c r="B86" s="64"/>
       <c r="C86" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D86" s="38"/>
       <c r="E86" s="39" t="s">
@@ -4442,8 +4566,9 @@
       <c r="I86" s="38">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="104"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
         <v>210</v>
       </c>
@@ -4460,13 +4585,14 @@
         <v>137</v>
       </c>
       <c r="H87" s="81" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I87" s="38">
         <v>481.8</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" s="104"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
         <v>210</v>
       </c>
@@ -4486,8 +4612,9 @@
         <v>144</v>
       </c>
       <c r="I88" s="38"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" s="104"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="64" t="s">
         <v>210</v>
       </c>
@@ -4509,8 +4636,9 @@
         <v>98</v>
       </c>
       <c r="I89" s="38"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" s="104"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="64" t="s">
         <v>210</v>
       </c>
@@ -4532,8 +4660,9 @@
         <v>174</v>
       </c>
       <c r="I90" s="38"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" s="104"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="64" t="s">
         <v>210</v>
       </c>
@@ -4555,8 +4684,9 @@
         <v>40</v>
       </c>
       <c r="I91" s="38"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" s="104"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="67" t="s">
         <v>26</v>
       </c>
@@ -4578,8 +4708,9 @@
         <v>1</v>
       </c>
       <c r="I92" s="42"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" s="105"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="67" t="s">
         <v>26</v>
       </c>
@@ -4599,8 +4730,9 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="I93" s="42"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" s="105"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="67" t="s">
         <v>26</v>
       </c>
@@ -4620,8 +4752,11 @@
         <v>178</v>
       </c>
       <c r="I94" s="42"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" s="105" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="67" t="s">
         <v>26</v>
       </c>
@@ -4643,8 +4778,11 @@
       <c r="I95" s="42">
         <v>63</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" s="105" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="67" t="s">
         <v>26</v>
       </c>
@@ -4666,8 +4804,11 @@
       <c r="I96" s="42">
         <v>739.8</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" s="105" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="67" t="s">
         <v>26</v>
       </c>
@@ -4689,8 +4830,9 @@
         <v>103</v>
       </c>
       <c r="I97" s="42"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" s="105"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="67" t="s">
         <v>26</v>
       </c>
@@ -4712,8 +4854,9 @@
         <v>180</v>
       </c>
       <c r="I98" s="42"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" s="105"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="67" t="s">
         <v>26</v>
       </c>
@@ -4735,8 +4878,9 @@
         <v>1</v>
       </c>
       <c r="I99" s="42"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" s="105"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="67" t="s">
         <v>26</v>
       </c>
@@ -4758,8 +4902,9 @@
         <v>184</v>
       </c>
       <c r="I100" s="42"/>
-    </row>
-    <row r="101" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J100" s="105"/>
+    </row>
+    <row r="101" spans="1:10" s="87" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="86" t="s">
         <v>223</v>
       </c>
@@ -4779,8 +4924,9 @@
       <c r="H101" s="90">
         <v>31</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" s="106"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="46" t="s">
         <v>223</v>
       </c>
@@ -4802,8 +4948,9 @@
         <v>186</v>
       </c>
       <c r="I102" s="47"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" s="107"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="46" t="s">
         <v>223</v>
       </c>
@@ -4820,11 +4967,12 @@
         <v>137</v>
       </c>
       <c r="H103" s="78" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="I103" s="47"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" s="107"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="46" t="s">
         <v>223</v>
       </c>
@@ -4841,11 +4989,12 @@
         <v>137</v>
       </c>
       <c r="H104" s="81" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="I104" s="47"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" s="107"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="46" t="s">
         <v>223</v>
       </c>
@@ -4862,15 +5011,16 @@
         <v>137</v>
       </c>
       <c r="H105" s="81" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="I105" s="47">
         <v>2034</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" s="107"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B106" s="65" t="s">
         <v>222</v>
@@ -4892,10 +5042,11 @@
         <v>187</v>
       </c>
       <c r="I106" s="51"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" s="108"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B107" s="65" t="s">
         <v>222</v>
@@ -4917,10 +5068,11 @@
         <v>5</v>
       </c>
       <c r="I107" s="74"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" s="109"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B108" s="65" t="s">
         <v>222</v>
@@ -4940,10 +5092,11 @@
         <v>140</v>
       </c>
       <c r="I108" s="51"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" s="108"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B109" s="65" t="s">
         <v>222</v>
@@ -4967,10 +5120,11 @@
       <c r="I109" s="53">
         <v>3000</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" s="110"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="65" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B110" s="65"/>
       <c r="C110" s="51" t="s">
@@ -4992,10 +5146,11 @@
       <c r="I110" s="53" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" s="110"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B111" s="65" t="s">
         <v>222</v>
@@ -5017,10 +5172,11 @@
       <c r="I111" s="53" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" s="110"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B112" s="65" t="s">
         <v>222</v>
@@ -5037,13 +5193,14 @@
         <v>137</v>
       </c>
       <c r="H112" s="79" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I112" s="53" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J112" s="110"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="65" t="s">
         <v>212</v>
       </c>
@@ -5063,13 +5220,14 @@
         <v>114</v>
       </c>
       <c r="I113" s="53"/>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J113" s="110"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="65" t="s">
         <v>211</v>
       </c>
       <c r="B114" s="65" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C114" s="51"/>
       <c r="D114" s="51"/>
@@ -5086,8 +5244,9 @@
         <v>160</v>
       </c>
       <c r="I114" s="53"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J114" s="110"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="77" t="s">
         <v>28</v>
       </c>
@@ -5109,10 +5268,11 @@
         <v>103</v>
       </c>
       <c r="I115" s="79"/>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J115" s="111"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="77" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B116" s="77"/>
       <c r="C116" s="83" t="s">
@@ -5132,10 +5292,11 @@
         <v>194</v>
       </c>
       <c r="I116" s="79"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J116" s="111"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="77" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B117" s="77"/>
       <c r="C117" s="83" t="s">
@@ -5155,8 +5316,9 @@
         <v>192</v>
       </c>
       <c r="I117" s="59"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J117" s="102"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="66" t="s">
         <v>31</v>
       </c>
@@ -5178,8 +5340,9 @@
       <c r="I118" s="54">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J118" s="112"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="66" t="s">
         <v>31</v>
       </c>
@@ -5199,18 +5362,15 @@
         <v>193</v>
       </c>
       <c r="I119" s="54"/>
-      <c r="K119">
-        <f ca="1">K119</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J119" s="112"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="66" t="s">
         <v>31</v>
       </c>
       <c r="B120" s="66"/>
       <c r="C120" s="54" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D120" s="54"/>
       <c r="E120" s="55" t="s">
@@ -5228,8 +5388,9 @@
       <c r="I120" s="54">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J120" s="112"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="66" t="s">
         <v>31</v>
       </c>
@@ -5246,13 +5407,16 @@
         <v>137</v>
       </c>
       <c r="H121" s="81" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I121" s="54">
         <v>1436</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J121" s="112" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="66" t="s">
         <v>31</v>
       </c>
@@ -5272,8 +5436,9 @@
         <v>111</v>
       </c>
       <c r="I122" s="54"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J122" s="112"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="66" t="s">
         <v>31</v>
       </c>
@@ -5293,6 +5458,7 @@
         <v>103</v>
       </c>
       <c r="I123" s="54"/>
+      <c r="J123" s="112"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5301,6 +5467,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F57573F99DE79145B2C4B20841E12603" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bffb4cedf0b3900262138fdae33e2dc4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0c1e910d-4918-42f1-af2c-ed1101d63abc" xmlns:ns4="786e620f-b1da-4f59-878c-ef7546d25bf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37173867f386110bdd2a41aaff59b7e1" ns3:_="" ns4:_="">
     <xsd:import namespace="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
@@ -5529,22 +5710,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE73DB8-1736-4671-8FD3-622DFFD73211}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D01498-1E58-48D4-ACAD-5E74F94105E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5561,29 +5752,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE73DB8-1736-4671-8FD3-622DFFD73211}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated for changes for GE data
</commit_message>
<xml_diff>
--- a/config/ukrin_conf.xlsx
+++ b/config/ukrin_conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\martin\code\xnat-dicomqc\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B141FAD-83E2-48C1-98AB-B31FF163F4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5BEB1F-BDE1-4D5E-9219-87E762A73658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="294">
   <si>
     <t>Vendors</t>
   </si>
@@ -602,9 +602,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>2049</t>
   </si>
   <si>
@@ -915,6 +912,12 @@
   </si>
   <si>
     <t>[3, 9]</t>
+  </si>
+  <si>
+    <t>[320, 600]</t>
+  </si>
+  <si>
+    <t>[45, 67.5]</t>
   </si>
 </sst>
 </file>
@@ -961,7 +964,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1064,12 +1067,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1083,7 +1080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1223,17 +1220,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1242,15 +1228,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1266,16 +1243,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1574,24 +1548,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1600,7 +1574,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1608,12 +1582,12 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1621,7 +1595,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1629,21 +1603,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
         <v>200</v>
-      </c>
-      <c r="B7" t="s">
-        <v>201</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
         <v>51</v>
@@ -1668,32 +1642,32 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,13 +1694,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1737,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,7 +1722,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,7 +1730,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1773,7 +1747,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,7 +1758,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,7 +1802,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1854,58 +1828,58 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="82" t="s">
-        <v>258</v>
+      <c r="A27" s="77" t="s">
+        <v>257</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="84" t="s">
-        <v>214</v>
+      <c r="D27" s="79" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="82" t="s">
-        <v>261</v>
+      <c r="A28" s="77" t="s">
+        <v>260</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="84" t="s">
-        <v>215</v>
+      <c r="D28" s="79" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="82" t="s">
-        <v>262</v>
+      <c r="A29" s="77" t="s">
+        <v>261</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="84" t="s">
-        <v>216</v>
+      <c r="D29" s="79" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="82" t="s">
-        <v>260</v>
+      <c r="A30" s="77" t="s">
+        <v>259</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="84" t="s">
-        <v>217</v>
+      <c r="D30" s="79" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="83" t="s">
-        <v>259</v>
+      <c r="A31" s="78" t="s">
+        <v>258</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="85" t="s">
-        <v>218</v>
+      <c r="D31" s="80" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1915,8 +1889,8 @@
       <c r="C32" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="85" t="s">
-        <v>222</v>
+      <c r="D32" s="80" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,41 +1900,41 @@
       <c r="C33" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="85" t="s">
+      <c r="D33" s="80" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="83" t="s">
-        <v>263</v>
+      <c r="A34" s="78" t="s">
+        <v>262</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="85" t="s">
-        <v>219</v>
+      <c r="D34" s="80" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="83" t="s">
-        <v>264</v>
+      <c r="A35" s="78" t="s">
+        <v>263</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="85" t="s">
-        <v>220</v>
+      <c r="D35" s="80" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="83" t="s">
-        <v>265</v>
+      <c r="A36" s="78" t="s">
+        <v>264</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="85" t="s">
-        <v>221</v>
+      <c r="D36" s="80" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,13 +1950,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,13 +1964,13 @@
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2007,7 +1981,7 @@
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,7 +2003,7 @@
         <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2040,7 +2014,7 @@
         <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2048,7 +2022,7 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C44" t="s">
         <v>33</v>
@@ -2065,7 +2039,7 @@
         <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2076,7 +2050,7 @@
         <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,7 +2094,7 @@
         <v>33</v>
       </c>
       <c r="D50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,7 +2105,7 @@
         <v>33</v>
       </c>
       <c r="D51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,27 +2116,27 @@
         <v>33</v>
       </c>
       <c r="D52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,7 +2147,7 @@
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,7 +2158,7 @@
         <v>33</v>
       </c>
       <c r="D58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2195,7 +2169,7 @@
         <v>33</v>
       </c>
       <c r="D59" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2206,7 +2180,7 @@
         <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2217,7 +2191,7 @@
         <v>33</v>
       </c>
       <c r="D61" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2248,7 +2222,7 @@
         <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,7 +2233,7 @@
         <v>51</v>
       </c>
       <c r="D65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2270,7 +2244,7 @@
         <v>51</v>
       </c>
       <c r="D66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2292,7 +2266,7 @@
         <v>51</v>
       </c>
       <c r="D68" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2303,7 +2277,7 @@
         <v>51</v>
       </c>
       <c r="D69" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,12 +2288,12 @@
         <v>51</v>
       </c>
       <c r="D70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C71" t="s">
         <v>51</v>
@@ -2341,7 +2315,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C73" t="s">
         <v>51</v>
@@ -2352,13 +2326,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C74" t="s">
         <v>51</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2369,7 +2343,7 @@
         <v>51</v>
       </c>
       <c r="D75" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,7 +2354,7 @@
         <v>51</v>
       </c>
       <c r="D76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2402,7 +2376,7 @@
         <v>51</v>
       </c>
       <c r="D78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,7 +2387,7 @@
         <v>51</v>
       </c>
       <c r="D79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2424,7 +2398,7 @@
         <v>51</v>
       </c>
       <c r="D80" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2435,18 +2409,18 @@
         <v>51</v>
       </c>
       <c r="D81" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C82" t="s">
         <v>51</v>
       </c>
       <c r="D82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2457,7 +2431,7 @@
         <v>51</v>
       </c>
       <c r="D83" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2479,7 +2453,7 @@
         <v>51</v>
       </c>
       <c r="D85" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2490,7 +2464,7 @@
         <v>51</v>
       </c>
       <c r="D86" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2501,7 +2475,7 @@
         <v>51</v>
       </c>
       <c r="D87" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2512,11 +2486,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L123"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2537,10 +2511,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2563,16 +2537,16 @@
       <c r="I1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="93" t="s">
-        <v>288</v>
+      <c r="J1" s="83" t="s">
+        <v>287</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" s="72"/>
       <c r="C2" t="s">
@@ -2593,10 +2567,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
-        <v>287</v>
-      </c>
-      <c r="B3" s="91" t="s">
-        <v>222</v>
+        <v>286</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>221</v>
       </c>
       <c r="C3" t="s">
         <v>81</v>
@@ -2616,10 +2590,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
-        <v>291</v>
-      </c>
-      <c r="B4" s="91" t="s">
-        <v>222</v>
+        <v>290</v>
+      </c>
+      <c r="B4" s="81" t="s">
+        <v>221</v>
       </c>
       <c r="C4" t="s">
         <v>83</v>
@@ -2637,13 +2611,13 @@
         <v>5</v>
       </c>
       <c r="K4" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L4" s="60"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" t="s">
@@ -2664,7 +2638,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" t="s">
@@ -2682,14 +2656,14 @@
       <c r="H6" s="5">
         <v>5</v>
       </c>
-      <c r="K6" s="83" t="s">
+      <c r="K6" s="78" t="s">
         <v>90</v>
       </c>
       <c r="L6" s="59"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" t="s">
@@ -2710,10 +2684,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
-        <v>232</v>
-      </c>
-      <c r="B8" s="91" t="s">
-        <v>222</v>
+        <v>231</v>
+      </c>
+      <c r="B8" s="81" t="s">
+        <v>221</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>92</v>
@@ -2730,7 +2704,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B9" s="72"/>
       <c r="E9" s="2" t="s">
@@ -2748,7 +2722,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10" s="3"/>
       <c r="E10" s="2" t="s">
@@ -2766,7 +2740,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B11" s="72"/>
       <c r="E11" s="2" t="s">
@@ -2807,28 +2781,26 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="83" t="s">
+      <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="83"/>
-      <c r="E13" s="79" t="s">
+      <c r="E13" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="83" t="s">
+      <c r="F13" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="81" t="s">
-        <v>277</v>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" t="s">
+        <v>276</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K13" t="s">
         <v>100</v>
@@ -2836,7 +2808,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" t="s">
@@ -2854,21 +2826,20 @@
       <c r="H14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="K14" s="34" t="s">
+      <c r="K14" t="s">
         <v>104</v>
       </c>
-      <c r="L14" s="34"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B15" s="72"/>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F15" t="s">
         <v>102</v>
@@ -2877,14 +2848,12 @@
         <v>79</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
+        <v>270</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" t="s">
@@ -2902,14 +2871,13 @@
       <c r="H16" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="34" t="s">
+      <c r="K16" t="s">
         <v>104</v>
       </c>
-      <c r="L16" s="34"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" t="s">
@@ -2927,15 +2895,13 @@
       <c r="H17" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B18" s="72"/>
-      <c r="C18" s="92" t="s">
+      <c r="C18" s="82" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="10" t="s">
@@ -2951,12 +2917,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B19" s="72"/>
-      <c r="C19" s="92" t="s">
+      <c r="C19" s="82" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -2972,12 +2938,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B20" s="72"/>
-      <c r="C20" s="92" t="s">
+      <c r="C20" s="82" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -2993,16 +2959,16 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B21" s="72"/>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="82" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F21" t="s">
         <v>117</v>
@@ -3014,16 +2980,16 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B22" s="72"/>
-      <c r="C22" s="92" t="s">
+      <c r="C22" s="82" t="s">
         <v>51</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F22" t="s">
         <v>117</v>
@@ -3035,12 +3001,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
         <v>118</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="69"/>
@@ -3057,11 +3023,11 @@
         <v>121</v>
       </c>
       <c r="I23" s="69"/>
-      <c r="J23" s="94"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J23" s="84"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="6" t="s">
@@ -3081,11 +3047,11 @@
         <v>12</v>
       </c>
       <c r="I24" s="6"/>
-      <c r="J24" s="95"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J24" s="85"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="6" t="s">
@@ -3105,15 +3071,15 @@
         <v>12</v>
       </c>
       <c r="I25" s="6"/>
-      <c r="J25" s="95"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J25" s="85"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="11" t="s">
@@ -3129,11 +3095,11 @@
         <v>129</v>
       </c>
       <c r="I26" s="6"/>
-      <c r="J26" s="95"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J26" s="85"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="6" t="s">
@@ -3150,14 +3116,14 @@
         <v>128</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I27" s="6"/>
-      <c r="J27" s="95"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J27" s="85"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="6"/>
@@ -3175,11 +3141,11 @@
         <v>132</v>
       </c>
       <c r="I28" s="6"/>
-      <c r="J28" s="95"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J28" s="85"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="6"/>
@@ -3197,11 +3163,11 @@
         <v>80</v>
       </c>
       <c r="I29" s="6"/>
-      <c r="J29" s="95"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J29" s="85"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="6"/>
@@ -3221,9 +3187,9 @@
       <c r="I30" s="6">
         <v>299.60000000000002</v>
       </c>
-      <c r="J30" s="95"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J30" s="85"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>23</v>
       </c>
@@ -3245,9 +3211,9 @@
         <v>4.5</v>
       </c>
       <c r="I31" s="12"/>
-      <c r="J31" s="96"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J31" s="86"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>23</v>
       </c>
@@ -3269,7 +3235,7 @@
         <v>10</v>
       </c>
       <c r="I32" s="12"/>
-      <c r="J32" s="96"/>
+      <c r="J32" s="86"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
@@ -3293,7 +3259,7 @@
         <v>10</v>
       </c>
       <c r="I33" s="12"/>
-      <c r="J33" s="96"/>
+      <c r="J33" s="86"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
@@ -3315,7 +3281,7 @@
         <v>139</v>
       </c>
       <c r="I34" s="12"/>
-      <c r="J34" s="96"/>
+      <c r="J34" s="86"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
@@ -3323,7 +3289,7 @@
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="15" t="s">
@@ -3339,7 +3305,7 @@
         <v>140</v>
       </c>
       <c r="I35" s="12"/>
-      <c r="J35" s="96"/>
+      <c r="J35" s="86"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
@@ -3363,7 +3329,7 @@
         <v>141</v>
       </c>
       <c r="I36" s="12"/>
-      <c r="J36" s="96"/>
+      <c r="J36" s="86"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
@@ -3387,7 +3353,7 @@
       <c r="I37" s="12">
         <v>299.60000000000002</v>
       </c>
-      <c r="J37" s="96"/>
+      <c r="J37" s="86"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
@@ -3411,7 +3377,7 @@
         <v>143</v>
       </c>
       <c r="I38" s="12"/>
-      <c r="J38" s="96"/>
+      <c r="J38" s="86"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
@@ -3435,7 +3401,7 @@
         <v>144</v>
       </c>
       <c r="I39" s="12"/>
-      <c r="J39" s="96"/>
+      <c r="J39" s="86"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
@@ -3447,7 +3413,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>102</v>
@@ -3456,10 +3422,10 @@
         <v>79</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I40" s="12"/>
-      <c r="J40" s="96"/>
+      <c r="J40" s="86"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
@@ -3483,7 +3449,7 @@
         <v>145</v>
       </c>
       <c r="I41" s="12"/>
-      <c r="J41" s="96"/>
+      <c r="J41" s="86"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
@@ -3507,7 +3473,7 @@
         <v>5</v>
       </c>
       <c r="I42" s="12"/>
-      <c r="J42" s="96"/>
+      <c r="J42" s="86"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="61" t="s">
@@ -3529,7 +3495,7 @@
         <v>147</v>
       </c>
       <c r="I43" s="18"/>
-      <c r="J43" s="97"/>
+      <c r="J43" s="87"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="61" t="s">
@@ -3551,7 +3517,7 @@
         <v>155</v>
       </c>
       <c r="I44" s="18"/>
-      <c r="J44" s="97"/>
+      <c r="J44" s="87"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="61" t="s">
@@ -3575,7 +3541,7 @@
       <c r="I45" s="18">
         <v>787.5</v>
       </c>
-      <c r="J45" s="97"/>
+      <c r="J45" s="87"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="61" t="s">
@@ -3597,7 +3563,7 @@
         <v>110</v>
       </c>
       <c r="I46" s="18"/>
-      <c r="J46" s="97"/>
+      <c r="J46" s="87"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="61" t="s">
@@ -3621,7 +3587,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I47" s="18"/>
-      <c r="J47" s="97"/>
+      <c r="J47" s="87"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="61" t="s">
@@ -3645,9 +3611,9 @@
         <v>2.46</v>
       </c>
       <c r="I48" s="18"/>
-      <c r="J48" s="97"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J48" s="87"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="61" t="s">
         <v>19</v>
       </c>
@@ -3669,9 +3635,9 @@
         <v>17</v>
       </c>
       <c r="I49" s="18"/>
-      <c r="J49" s="97"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J49" s="87"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="61" t="s">
         <v>19</v>
       </c>
@@ -3693,9 +3659,9 @@
         <v>17</v>
       </c>
       <c r="I50" s="18"/>
-      <c r="J50" s="97"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J50" s="87"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="61" t="s">
         <v>19</v>
       </c>
@@ -3717,13 +3683,12 @@
         <v>152</v>
       </c>
       <c r="I51" s="18"/>
-      <c r="J51" s="97"/>
-      <c r="K51" s="34" t="s">
+      <c r="J51" s="87"/>
+      <c r="K51" t="s">
         <v>153</v>
       </c>
-      <c r="L51" s="34"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="61" t="s">
         <v>19</v>
       </c>
@@ -3745,9 +3710,9 @@
         <v>154</v>
       </c>
       <c r="I52" s="18"/>
-      <c r="J52" s="97"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J52" s="87"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="62" t="s">
         <v>21</v>
       </c>
@@ -3769,9 +3734,9 @@
         <v>140</v>
       </c>
       <c r="I53" s="22"/>
-      <c r="J53" s="98"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J53" s="88"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="62" t="s">
         <v>21</v>
       </c>
@@ -3793,9 +3758,9 @@
       <c r="I54" s="22">
         <v>877</v>
       </c>
-      <c r="J54" s="98"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J54" s="88"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="62" t="s">
         <v>21</v>
       </c>
@@ -3817,9 +3782,9 @@
       <c r="I55" s="22">
         <v>787.5</v>
       </c>
-      <c r="J55" s="98"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J55" s="88"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="62" t="s">
         <v>21</v>
       </c>
@@ -3841,9 +3806,9 @@
       <c r="I56" s="22">
         <v>61</v>
       </c>
-      <c r="J56" s="98"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J56" s="88"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="62" t="s">
         <v>21</v>
       </c>
@@ -3865,9 +3830,9 @@
         <v>60</v>
       </c>
       <c r="I57" s="22"/>
-      <c r="J57" s="98"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J57" s="88"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="62" t="s">
         <v>21</v>
       </c>
@@ -3891,9 +3856,9 @@
       <c r="I58" s="22">
         <v>62</v>
       </c>
-      <c r="J58" s="98"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J58" s="88"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="62" t="s">
         <v>21</v>
       </c>
@@ -3915,9 +3880,9 @@
         <v>17</v>
       </c>
       <c r="I59" s="22"/>
-      <c r="J59" s="98"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J59" s="88"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="62" t="s">
         <v>21</v>
       </c>
@@ -3939,9 +3904,9 @@
         <v>17</v>
       </c>
       <c r="I60" s="22"/>
-      <c r="J60" s="98"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J60" s="88"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="62" t="s">
         <v>21</v>
       </c>
@@ -3963,13 +3928,12 @@
         <v>152</v>
       </c>
       <c r="I61" s="22"/>
-      <c r="J61" s="98"/>
-      <c r="K61" s="34" t="s">
+      <c r="J61" s="88"/>
+      <c r="K61" t="s">
         <v>153</v>
       </c>
-      <c r="L61" s="34"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="62" t="s">
         <v>21</v>
       </c>
@@ -3991,11 +3955,11 @@
         <v>145</v>
       </c>
       <c r="I62" s="22"/>
-      <c r="J62" s="98"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J62" s="88"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B63" s="58"/>
       <c r="C63" s="26"/>
@@ -4013,11 +3977,11 @@
         <v>140</v>
       </c>
       <c r="I63" s="26"/>
-      <c r="J63" s="99"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J63" s="89"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B64" s="58"/>
       <c r="C64" s="27" t="s">
@@ -4039,11 +4003,11 @@
       <c r="I64" s="27">
         <v>3000</v>
       </c>
-      <c r="J64" s="100"/>
+      <c r="J64" s="90"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B65" s="58"/>
       <c r="C65" s="27"/>
@@ -4063,14 +4027,16 @@
       <c r="I65" s="27">
         <v>1988</v>
       </c>
-      <c r="J65" s="100"/>
+      <c r="J65" s="90"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B66" s="58"/>
-      <c r="C66" s="27"/>
+      <c r="C66" s="27" t="s">
+        <v>107</v>
+      </c>
       <c r="D66" s="27"/>
       <c r="E66" s="27" t="s">
         <v>126</v>
@@ -4082,48 +4048,50 @@
         <v>137</v>
       </c>
       <c r="H66" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I66" s="27">
         <v>65</v>
       </c>
-      <c r="J66" s="100"/>
+      <c r="J66" s="90"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="58" t="s">
-        <v>284</v>
+        <v>228</v>
       </c>
       <c r="B67" s="58"/>
       <c r="C67" s="27" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D67" s="27"/>
       <c r="E67" s="27" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F67" s="27" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="G67" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="H67" s="27">
-        <v>13</v>
-      </c>
-      <c r="I67" s="27"/>
-      <c r="J67" s="100"/>
+        <v>137</v>
+      </c>
+      <c r="H67" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="I67" s="27">
+        <v>65</v>
+      </c>
+      <c r="J67" s="90"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="58" t="s">
-        <v>229</v>
+        <v>283</v>
       </c>
       <c r="B68" s="58"/>
       <c r="C68" s="27" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="D68" s="27"/>
       <c r="E68" s="27" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>89</v>
@@ -4135,186 +4103,186 @@
         <v>13</v>
       </c>
       <c r="I68" s="27"/>
-      <c r="J68" s="100"/>
+      <c r="J68" s="90"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C69" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D69" s="30"/>
-      <c r="E69" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="F69" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="G69" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="H69" s="31">
-        <v>2</v>
-      </c>
-      <c r="I69" s="30"/>
-      <c r="J69" s="101"/>
+      <c r="A69" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="B69" s="58"/>
+      <c r="C69" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F69" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G69" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H69" s="27">
+        <v>13</v>
+      </c>
+      <c r="I69" s="27"/>
+      <c r="J69" s="90"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="65" t="s">
-        <v>222</v>
+      <c r="B70" s="29" t="s">
+        <v>221</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="33" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F70" s="30" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G70" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="H70" s="31" t="s">
-        <v>158</v>
+        <v>79</v>
+      </c>
+      <c r="H70" s="31">
+        <v>2</v>
       </c>
       <c r="I70" s="30"/>
-      <c r="J70" s="101"/>
+      <c r="J70" s="91"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C71" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" s="83"/>
-      <c r="E71" s="78" t="s">
+      <c r="B71" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" s="30"/>
+      <c r="E71" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="F71" s="83" t="s">
+      <c r="F71" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="G71" s="79" t="s">
+      <c r="G71" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="H71" s="81" t="s">
-        <v>268</v>
+      <c r="H71" s="31" t="s">
+        <v>158</v>
       </c>
       <c r="I71" s="30"/>
-      <c r="J71" s="101"/>
+      <c r="J71" s="91"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B72" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C72" s="83"/>
-      <c r="D72" s="83"/>
-      <c r="E72" s="78" t="s">
+      <c r="B72" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="30"/>
+      <c r="E72" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G72" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="H72" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="I72" s="30"/>
+      <c r="J72" s="30"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="F72" s="83" t="s">
+      <c r="F73" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="G72" s="79" t="s">
+      <c r="G73" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="H72" s="78" t="s">
-        <v>278</v>
-      </c>
-      <c r="I72" s="30"/>
-      <c r="J72" s="101"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C73" s="59"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="78" t="s">
-        <v>133</v>
-      </c>
-      <c r="F73" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="G73" s="79" t="s">
-        <v>185</v>
-      </c>
-      <c r="H73" s="81" t="s">
-        <v>205</v>
-      </c>
-      <c r="I73" s="59"/>
-      <c r="J73" s="102"/>
-      <c r="K73" t="s">
-        <v>206</v>
-      </c>
+      <c r="H73" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="I73" s="30"/>
+      <c r="J73" s="30"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B74" s="65" t="s">
-        <v>222</v>
+      <c r="B74" s="29" t="s">
+        <v>221</v>
       </c>
       <c r="C74" s="30"/>
       <c r="D74" s="30"/>
-      <c r="E74" s="33" t="s">
+      <c r="E74" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="F74" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G74" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H74" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="I74" s="30"/>
+      <c r="J74" s="30"/>
+      <c r="K74" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="30" t="s">
+      <c r="F75" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="32" t="s">
+      <c r="G75" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="H74" s="31" t="s">
+      <c r="H75" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="I74" s="30">
+      <c r="I75" s="30">
         <v>787.5</v>
       </c>
-      <c r="J74" s="101"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="B75" s="63"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="F75" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G75" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="H75" s="35" t="s">
-        <v>159</v>
-      </c>
-      <c r="I75" s="34">
-        <v>1.68</v>
-      </c>
-      <c r="J75" s="103"/>
+      <c r="J75" s="91"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="63" t="s">
@@ -4324,19 +4292,21 @@
       <c r="C76" s="34"/>
       <c r="D76" s="34"/>
       <c r="E76" s="37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F76" s="34" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G76" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H76" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="I76" s="34"/>
-      <c r="J76" s="103"/>
+        <v>137</v>
+      </c>
+      <c r="H76" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="I76" s="34">
+        <v>1.68</v>
+      </c>
+      <c r="J76" s="92"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="63" t="s">
@@ -4346,21 +4316,19 @@
       <c r="C77" s="34"/>
       <c r="D77" s="34"/>
       <c r="E77" s="37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F77" s="34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G77" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="H77" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="I77" s="34">
-        <v>3.4</v>
-      </c>
-      <c r="J77" s="103"/>
+        <v>79</v>
+      </c>
+      <c r="H77" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="I77" s="34"/>
+      <c r="J77" s="92"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="63" t="s">
@@ -4370,109 +4338,111 @@
       <c r="C78" s="34"/>
       <c r="D78" s="34"/>
       <c r="E78" s="37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F78" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G78" s="36" t="s">
         <v>137</v>
       </c>
       <c r="H78" s="35" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="I78" s="34">
-        <v>787.5</v>
-      </c>
-      <c r="J78" s="103"/>
-    </row>
-    <row r="79" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3.4</v>
+      </c>
+      <c r="J78" s="92"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="63" t="s">
         <v>9</v>
       </c>
       <c r="B79" s="63"/>
-      <c r="C79" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="C79" s="34"/>
       <c r="D79" s="34"/>
-      <c r="E79" s="36" t="s">
-        <v>162</v>
+      <c r="E79" s="37" t="s">
+        <v>135</v>
       </c>
       <c r="F79" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="G79" s="36"/>
-      <c r="H79" s="35"/>
-      <c r="I79" s="34"/>
-      <c r="J79" s="103"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="G79" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="H79" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="I79" s="34">
+        <v>787.5</v>
+      </c>
+      <c r="J79" s="92"/>
+    </row>
+    <row r="80" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="63" t="s">
         <v>9</v>
       </c>
       <c r="B80" s="63"/>
-      <c r="C80" s="34"/>
+      <c r="C80" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="D80" s="34"/>
-      <c r="E80" s="37" t="s">
-        <v>164</v>
+      <c r="E80" s="36" t="s">
+        <v>162</v>
       </c>
       <c r="F80" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="G80" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H80" s="35">
-        <v>60</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="G80" s="36"/>
+      <c r="H80" s="35"/>
       <c r="I80" s="34"/>
-      <c r="J80" s="103"/>
+      <c r="J80" s="92"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="63" t="s">
         <v>9</v>
       </c>
       <c r="B81" s="63"/>
-      <c r="C81" s="34" t="s">
-        <v>2</v>
-      </c>
+      <c r="C81" s="34"/>
       <c r="D81" s="34"/>
       <c r="E81" s="37" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F81" s="34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G81" s="36" t="s">
         <v>79</v>
       </c>
       <c r="H81" s="35">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="I81" s="34"/>
-      <c r="J81" s="103"/>
+      <c r="J81" s="92"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="63" t="s">
         <v>9</v>
       </c>
       <c r="B82" s="63"/>
-      <c r="C82" s="34"/>
+      <c r="C82" s="34" t="s">
+        <v>2</v>
+      </c>
       <c r="D82" s="34"/>
       <c r="E82" s="37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F82" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G82" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="H82" s="35" t="s">
-        <v>202</v>
+        <v>79</v>
+      </c>
+      <c r="H82" s="35">
+        <v>1000</v>
       </c>
       <c r="I82" s="34"/>
-      <c r="J82" s="103"/>
+      <c r="J82" s="92"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="63" t="s">
@@ -4481,331 +4451,329 @@
       <c r="B83" s="63"/>
       <c r="C83" s="34"/>
       <c r="D83" s="34"/>
-      <c r="E83" s="36" t="s">
+      <c r="E83" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="F83" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="G83" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="H83" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="I83" s="34"/>
+      <c r="J83" s="92"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" s="63"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="F83" s="34" t="s">
+      <c r="F84" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="G83" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H83" s="35">
+      <c r="G84" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="H84" s="35">
         <v>8</v>
       </c>
-      <c r="I83" s="34"/>
-      <c r="J83" s="103"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="64" t="s">
-        <v>210</v>
-      </c>
-      <c r="B84" s="64"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="F84" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="G84" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="H84" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="I84" s="38">
-        <v>3.3</v>
-      </c>
-      <c r="J84" s="104"/>
+      <c r="I84" s="34"/>
+      <c r="J84" s="92"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B85" s="64"/>
       <c r="C85" s="38"/>
       <c r="D85" s="38"/>
       <c r="E85" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F85" s="38" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G85" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H85" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="I85" s="38"/>
-      <c r="J85" s="104"/>
+        <v>137</v>
+      </c>
+      <c r="H85" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="I85" s="38">
+        <v>3.3</v>
+      </c>
+      <c r="J85" s="93"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B86" s="64"/>
-      <c r="C86" s="38" t="s">
-        <v>280</v>
-      </c>
+      <c r="C86" s="38"/>
       <c r="D86" s="38"/>
       <c r="E86" s="39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F86" s="38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G86" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="H86" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="I86" s="38">
-        <v>5.5</v>
-      </c>
-      <c r="J86" s="104"/>
+        <v>79</v>
+      </c>
+      <c r="H86" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="I86" s="38"/>
+      <c r="J86" s="93"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B87" s="64"/>
-      <c r="C87" s="38"/>
+      <c r="C87" s="38" t="s">
+        <v>279</v>
+      </c>
       <c r="D87" s="38"/>
       <c r="E87" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="F87" s="83" t="s">
-        <v>136</v>
-      </c>
-      <c r="G87" s="79" t="s">
+        <v>133</v>
+      </c>
+      <c r="F87" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G87" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="H87" s="81" t="s">
-        <v>276</v>
+      <c r="H87" s="41" t="s">
+        <v>172</v>
       </c>
       <c r="I87" s="38">
-        <v>481.8</v>
-      </c>
-      <c r="J87" s="104"/>
+        <v>5.5</v>
+      </c>
+      <c r="J87" s="93"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B88" s="64"/>
-      <c r="C88" s="38"/>
+      <c r="C88" s="38" t="s">
+        <v>107</v>
+      </c>
       <c r="D88" s="38"/>
       <c r="E88" s="39" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="F88" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="G88" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H88" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="I88" s="38"/>
-      <c r="J88" s="104"/>
+        <v>136</v>
+      </c>
+      <c r="G88" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="H88" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="I88" s="38">
+        <v>481.8</v>
+      </c>
+      <c r="J88" s="93"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B89" s="64"/>
       <c r="C89" s="38" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="D89" s="38"/>
       <c r="E89" s="39" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="F89" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="G89" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H89" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="I89" s="38"/>
-      <c r="J89" s="104"/>
+        <v>136</v>
+      </c>
+      <c r="G89" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="H89" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="I89" s="38">
+        <v>481.8</v>
+      </c>
+      <c r="J89" s="93"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B90" s="64"/>
-      <c r="C90" s="38" t="s">
-        <v>51</v>
-      </c>
+      <c r="C90" s="38"/>
       <c r="D90" s="38"/>
       <c r="E90" s="39" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
       <c r="F90" s="38" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G90" s="40" t="s">
         <v>79</v>
       </c>
       <c r="H90" s="39" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I90" s="38"/>
-      <c r="J90" s="104"/>
+      <c r="J90" s="93"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B91" s="64"/>
       <c r="C91" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D91" s="38"/>
+      <c r="E91" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F91" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G91" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H91" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="I91" s="38"/>
+      <c r="J91" s="93"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="64" t="s">
+        <v>209</v>
+      </c>
+      <c r="B92" s="64"/>
+      <c r="C92" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D92" s="38"/>
+      <c r="E92" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F92" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G92" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H92" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I92" s="38"/>
+      <c r="J92" s="93"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="64" t="s">
+        <v>209</v>
+      </c>
+      <c r="B93" s="64"/>
+      <c r="C93" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D91" s="38"/>
-      <c r="E91" s="40" t="s">
+      <c r="D93" s="38"/>
+      <c r="E93" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="F91" s="38" t="s">
+      <c r="F93" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="G91" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H91" s="41">
+      <c r="G93" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H93" s="41">
         <v>40</v>
       </c>
-      <c r="I91" s="38"/>
-      <c r="J91" s="104"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="67"/>
-      <c r="C92" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D92" s="42"/>
-      <c r="E92" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="F92" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="G92" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H92" s="45">
-        <v>1</v>
-      </c>
-      <c r="I92" s="42"/>
-      <c r="J92" s="105"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B93" s="67"/>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
-      <c r="E93" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="F93" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="G93" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H93" s="45">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="I93" s="42"/>
-      <c r="J93" s="105"/>
+      <c r="I93" s="38"/>
+      <c r="J93" s="93"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B94" s="67"/>
-      <c r="C94" s="42"/>
+      <c r="C94" s="42" t="s">
+        <v>2</v>
+      </c>
       <c r="D94" s="42"/>
       <c r="E94" s="43" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
       <c r="F94" s="42" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="G94" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H94" s="43" t="s">
-        <v>178</v>
+      <c r="H94" s="45">
+        <v>1</v>
       </c>
       <c r="I94" s="42"/>
-      <c r="J94" s="105" t="s">
-        <v>289</v>
-      </c>
+      <c r="J94" s="94"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B95" s="67"/>
-      <c r="C95" s="43"/>
-      <c r="D95" s="43"/>
+      <c r="C95" s="42"/>
+      <c r="D95" s="42"/>
       <c r="E95" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="F95" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="G95" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="H95" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="I95" s="42">
-        <v>63</v>
-      </c>
-      <c r="J95" s="105" t="s">
-        <v>289</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F95" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="G95" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H95" s="45">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I95" s="42"/>
+      <c r="J95" s="94"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B96" s="67"/>
-      <c r="C96" s="43"/>
-      <c r="D96" s="43"/>
+      <c r="C96" s="42"/>
+      <c r="D96" s="42"/>
       <c r="E96" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="F96" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="G96" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="H96" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="I96" s="42">
-        <v>739.8</v>
-      </c>
-      <c r="J96" s="105" t="s">
-        <v>289</v>
+        <v>130</v>
+      </c>
+      <c r="F96" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="G96" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H96" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="I96" s="42"/>
+      <c r="J96" s="94" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -4813,571 +4781,577 @@
         <v>26</v>
       </c>
       <c r="B97" s="67"/>
-      <c r="C97" s="43" t="s">
-        <v>2</v>
-      </c>
+      <c r="C97" s="43"/>
       <c r="D97" s="43"/>
       <c r="E97" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="F97" s="42" t="s">
-        <v>102</v>
+        <v>133</v>
+      </c>
+      <c r="F97" s="43" t="s">
+        <v>134</v>
       </c>
       <c r="G97" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="H97" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="I97" s="42"/>
-      <c r="J97" s="105"/>
+        <v>137</v>
+      </c>
+      <c r="H97" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="I97" s="42">
+        <v>63</v>
+      </c>
+      <c r="J97" s="94" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B98" s="67"/>
-      <c r="C98" s="43" t="s">
-        <v>51</v>
-      </c>
+      <c r="C98" s="43"/>
       <c r="D98" s="43"/>
       <c r="E98" s="43" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="F98" s="43" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="G98" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="H98" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="I98" s="42"/>
-      <c r="J98" s="105"/>
+        <v>137</v>
+      </c>
+      <c r="H98" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="I98" s="42">
+        <v>739.8</v>
+      </c>
+      <c r="J98" s="94" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B99" s="67"/>
-      <c r="C99" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D99" s="42"/>
-      <c r="E99" s="44" t="s">
-        <v>181</v>
+      <c r="C99" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="43"/>
+      <c r="E99" s="43" t="s">
+        <v>101</v>
       </c>
       <c r="F99" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="G99" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H99" s="45">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="G99" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="H99" s="43" t="s">
+        <v>103</v>
       </c>
       <c r="I99" s="42"/>
-      <c r="J99" s="105"/>
+      <c r="J99" s="94"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B100" s="67"/>
-      <c r="C100" s="42" t="s">
+      <c r="C100" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D100" s="43"/>
+      <c r="E100" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F100" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G100" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="H100" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="I100" s="42"/>
+      <c r="J100" s="94"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="67"/>
+      <c r="C101" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D101" s="42"/>
+      <c r="E101" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="F101" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G101" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H101" s="45">
+        <v>1</v>
+      </c>
+      <c r="I101" s="42"/>
+      <c r="J101" s="94"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="67"/>
+      <c r="C102" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D100" s="42"/>
-      <c r="E100" s="43" t="s">
+      <c r="D102" s="42"/>
+      <c r="E102" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="F100" s="42" t="s">
+      <c r="F102" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="G100" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H100" s="45" t="s">
+      <c r="G102" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H102" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="I100" s="42"/>
-      <c r="J100" s="105"/>
-    </row>
-    <row r="101" spans="1:10" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="86" t="s">
-        <v>223</v>
-      </c>
-      <c r="B101" s="86"/>
-      <c r="C101" s="87" t="s">
-        <v>2</v>
-      </c>
-      <c r="E101" s="88" t="s">
-        <v>88</v>
-      </c>
-      <c r="F101" s="87" t="s">
-        <v>89</v>
-      </c>
-      <c r="G101" s="89" t="s">
-        <v>79</v>
-      </c>
-      <c r="H101" s="90">
-        <v>31</v>
-      </c>
-      <c r="J101" s="106"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="B102" s="46"/>
-      <c r="C102" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D102" s="47"/>
-      <c r="E102" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="F102" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="G102" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="H102" s="50" t="s">
-        <v>186</v>
-      </c>
-      <c r="I102" s="47"/>
-      <c r="J102" s="107"/>
+      <c r="I102" s="42"/>
+      <c r="J102" s="94"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B103" s="46"/>
-      <c r="C103" s="47"/>
+      <c r="C103" s="47" t="s">
+        <v>2</v>
+      </c>
       <c r="D103" s="47"/>
-      <c r="E103" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="F103" s="83" t="s">
-        <v>131</v>
-      </c>
-      <c r="G103" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="H103" s="78" t="s">
-        <v>292</v>
+      <c r="E103" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="F103" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="G103" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="H103" s="47">
+        <v>31</v>
       </c>
       <c r="I103" s="47"/>
-      <c r="J103" s="107"/>
+      <c r="J103" s="47"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B104" s="46"/>
-      <c r="C104" s="47"/>
+      <c r="C104" s="47" t="s">
+        <v>2</v>
+      </c>
       <c r="D104" s="47"/>
       <c r="E104" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="F104" s="83" t="s">
-        <v>134</v>
-      </c>
-      <c r="G104" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="H104" s="81" t="s">
-        <v>269</v>
+        <v>122</v>
+      </c>
+      <c r="F104" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="G104" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="H104" s="50" t="s">
+        <v>186</v>
       </c>
       <c r="I104" s="47"/>
-      <c r="J104" s="107"/>
+      <c r="J104" s="95"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B105" s="46"/>
       <c r="C105" s="47"/>
       <c r="D105" s="47"/>
       <c r="E105" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="F105" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="G105" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H105" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="I105" s="47"/>
+      <c r="J105" s="95"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B106" s="46"/>
+      <c r="C106" s="47"/>
+      <c r="D106" s="47"/>
+      <c r="E106" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="F106" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="G106" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H106" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="I106" s="47"/>
+      <c r="J106" s="95"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B107" s="46"/>
+      <c r="C107" s="47"/>
+      <c r="D107" s="47"/>
+      <c r="E107" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="F105" s="83" t="s">
+      <c r="F107" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="G105" s="79" t="s">
+      <c r="G107" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="H105" s="81" t="s">
-        <v>274</v>
-      </c>
-      <c r="I105" s="47">
+      <c r="H107" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="I107" s="47">
         <v>2034</v>
       </c>
-      <c r="J105" s="107"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="65" t="s">
-        <v>237</v>
-      </c>
-      <c r="B106" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C106" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D106" s="51"/>
-      <c r="E106" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="F106" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="G106" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="H106" s="52" t="s">
-        <v>187</v>
-      </c>
-      <c r="I106" s="51"/>
-      <c r="J106" s="108"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="65" t="s">
-        <v>237</v>
-      </c>
-      <c r="B107" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C107" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="D107" s="74"/>
-      <c r="E107" s="75" t="s">
-        <v>91</v>
-      </c>
-      <c r="F107" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="G107" s="75" t="s">
-        <v>79</v>
-      </c>
-      <c r="H107" s="76">
-        <v>5</v>
-      </c>
-      <c r="I107" s="74"/>
-      <c r="J107" s="109"/>
+      <c r="J107" s="95"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="65" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B108" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C108" s="51"/>
+        <v>221</v>
+      </c>
+      <c r="C108" s="51" t="s">
+        <v>2</v>
+      </c>
       <c r="D108" s="51"/>
       <c r="E108" s="52" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
       <c r="F108" s="51" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="G108" s="53" t="s">
         <v>79</v>
       </c>
       <c r="H108" s="52" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="I108" s="51"/>
-      <c r="J108" s="108"/>
+      <c r="J108" s="96"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="65" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B109" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C109" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="D109" s="51"/>
-      <c r="E109" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="F109" s="53" t="s">
-        <v>134</v>
-      </c>
-      <c r="G109" s="53" t="s">
-        <v>137</v>
-      </c>
-      <c r="H109" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="I109" s="53">
-        <v>3000</v>
-      </c>
-      <c r="J109" s="110"/>
+        <v>221</v>
+      </c>
+      <c r="C109" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D109" s="74"/>
+      <c r="E109" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="F109" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="G109" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="H109" s="76">
+        <v>5</v>
+      </c>
+      <c r="I109" s="74"/>
+      <c r="J109" s="97"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="65" t="s">
-        <v>238</v>
-      </c>
-      <c r="B110" s="65"/>
-      <c r="C110" s="51" t="s">
-        <v>51</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="B110" s="65" t="s">
+        <v>221</v>
+      </c>
+      <c r="C110" s="51"/>
       <c r="D110" s="51"/>
-      <c r="E110" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="F110" s="53" t="s">
-        <v>134</v>
+      <c r="E110" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F110" s="51" t="s">
+        <v>131</v>
       </c>
       <c r="G110" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="H110" s="53" t="s">
-        <v>188</v>
-      </c>
-      <c r="I110" s="53" t="s">
-        <v>188</v>
-      </c>
-      <c r="J110" s="110"/>
+      <c r="H110" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="I110" s="51"/>
+      <c r="J110" s="96"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="65" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B111" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C111" s="51"/>
+        <v>221</v>
+      </c>
+      <c r="C111" s="51" t="s">
+        <v>107</v>
+      </c>
       <c r="D111" s="51"/>
       <c r="E111" s="53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F111" s="53" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G111" s="53" t="s">
         <v>137</v>
       </c>
       <c r="H111" s="53" t="s">
-        <v>157</v>
-      </c>
-      <c r="I111" s="53" t="s">
-        <v>189</v>
-      </c>
-      <c r="J111" s="110"/>
+        <v>141</v>
+      </c>
+      <c r="I111" s="53">
+        <v>3000</v>
+      </c>
+      <c r="J111" s="98"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="B112" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="C112" s="51"/>
+      <c r="B112" s="65"/>
+      <c r="C112" s="51" t="s">
+        <v>51</v>
+      </c>
       <c r="D112" s="51"/>
-      <c r="E112" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="F112" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="G112" s="53" t="s">
+      <c r="E112" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="F112" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="G112" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="H112" s="79" t="s">
-        <v>273</v>
-      </c>
-      <c r="I112" s="53" t="s">
-        <v>190</v>
-      </c>
-      <c r="J112" s="110"/>
+      <c r="H112" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="I112" s="51">
+        <v>6000</v>
+      </c>
+      <c r="J112" s="51"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="65" t="s">
-        <v>212</v>
-      </c>
-      <c r="B113" s="65"/>
+        <v>236</v>
+      </c>
+      <c r="B113" s="65" t="s">
+        <v>221</v>
+      </c>
       <c r="C113" s="51"/>
       <c r="D113" s="51"/>
-      <c r="E113" s="52" t="s">
-        <v>119</v>
+      <c r="E113" s="51" t="s">
+        <v>135</v>
       </c>
       <c r="F113" s="51" t="s">
-        <v>191</v>
-      </c>
-      <c r="G113" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="H113" s="52" t="s">
-        <v>114</v>
-      </c>
-      <c r="I113" s="53"/>
-      <c r="J113" s="110"/>
+        <v>136</v>
+      </c>
+      <c r="G113" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="H113" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="I113" s="51" t="s">
+        <v>188</v>
+      </c>
+      <c r="J113" s="51"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="65" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="B114" s="65" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C114" s="51"/>
       <c r="D114" s="51"/>
-      <c r="E114" s="52" t="s">
+      <c r="E114" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="F114" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="G114" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="H114" s="51" t="s">
+        <v>272</v>
+      </c>
+      <c r="I114" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="J114" s="51"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="B115" s="65"/>
+      <c r="C115" s="51"/>
+      <c r="D115" s="51"/>
+      <c r="E115" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="F114" s="51" t="s">
+      <c r="F115" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="G115" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H115" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="I115" s="51"/>
+      <c r="J115" s="51"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="65" t="s">
+        <v>210</v>
+      </c>
+      <c r="B116" s="65" t="s">
+        <v>234</v>
+      </c>
+      <c r="C116" s="51"/>
+      <c r="D116" s="51"/>
+      <c r="E116" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F116" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="G116" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H116" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="I116" s="51"/>
+      <c r="J116" s="51"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117" s="65"/>
+      <c r="C117" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" s="51"/>
+      <c r="E117" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F117" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="G117" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H117" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="I117" s="51"/>
+      <c r="J117" s="51"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="65" t="s">
+        <v>239</v>
+      </c>
+      <c r="B118" s="65"/>
+      <c r="C118" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" s="51"/>
+      <c r="E118" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F118" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="G118" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H118" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="I118" s="51"/>
+      <c r="J118" s="51"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="65" t="s">
+        <v>235</v>
+      </c>
+      <c r="B119" s="65"/>
+      <c r="C119" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D119" s="51"/>
+      <c r="E119" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F119" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="G119" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H119" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="G114" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="H114" s="52" t="s">
-        <v>160</v>
-      </c>
-      <c r="I114" s="53"/>
-      <c r="J114" s="110"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="77" t="s">
-        <v>28</v>
-      </c>
-      <c r="B115" s="77"/>
-      <c r="C115" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="D115" s="59"/>
-      <c r="E115" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="F115" s="59" t="s">
-        <v>191</v>
-      </c>
-      <c r="G115" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="H115" s="78" t="s">
-        <v>103</v>
-      </c>
-      <c r="I115" s="79"/>
-      <c r="J115" s="111"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="77" t="s">
-        <v>240</v>
-      </c>
-      <c r="B116" s="77"/>
-      <c r="C116" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="D116" s="59"/>
-      <c r="E116" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="F116" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="G116" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="H116" s="78" t="s">
-        <v>194</v>
-      </c>
-      <c r="I116" s="79"/>
-      <c r="J116" s="111"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="77" t="s">
-        <v>236</v>
-      </c>
-      <c r="B117" s="77"/>
-      <c r="C117" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="D117" s="59"/>
-      <c r="E117" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="F117" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="G117" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="H117" s="78" t="s">
-        <v>192</v>
-      </c>
-      <c r="I117" s="59"/>
-      <c r="J117" s="102"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B118" s="66"/>
-      <c r="C118" s="54"/>
-      <c r="D118" s="54"/>
-      <c r="E118" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="F118" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="G118" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="H118" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="I118" s="54">
-        <v>2.5</v>
-      </c>
-      <c r="J118" s="112"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B119" s="66"/>
-      <c r="C119" s="54"/>
-      <c r="D119" s="54"/>
-      <c r="E119" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="F119" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="G119" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H119" s="55" t="s">
-        <v>193</v>
-      </c>
-      <c r="I119" s="54"/>
-      <c r="J119" s="112"/>
+      <c r="I119" s="51"/>
+      <c r="J119" s="51"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="66" t="s">
         <v>31</v>
       </c>
       <c r="B120" s="66"/>
-      <c r="C120" s="54" t="s">
-        <v>280</v>
-      </c>
+      <c r="C120" s="54"/>
       <c r="D120" s="54"/>
       <c r="E120" s="55" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F120" s="54" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G120" s="56" t="s">
         <v>137</v>
@@ -5386,9 +5360,9 @@
         <v>161</v>
       </c>
       <c r="I120" s="54">
-        <v>3.8</v>
-      </c>
-      <c r="J120" s="112"/>
+        <v>2.5</v>
+      </c>
+      <c r="J120" s="99"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="66" t="s">
@@ -5398,45 +5372,45 @@
       <c r="C121" s="54"/>
       <c r="D121" s="54"/>
       <c r="E121" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="F121" s="83" t="s">
-        <v>136</v>
-      </c>
-      <c r="G121" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="H121" s="81" t="s">
-        <v>275</v>
-      </c>
-      <c r="I121" s="54">
-        <v>1436</v>
-      </c>
-      <c r="J121" s="112" t="s">
-        <v>289</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F121" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="G121" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H121" s="55" t="s">
+        <v>192</v>
+      </c>
+      <c r="I121" s="54"/>
+      <c r="J121" s="99"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="66" t="s">
         <v>31</v>
       </c>
       <c r="B122" s="66"/>
-      <c r="C122" s="54"/>
+      <c r="C122" s="54" t="s">
+        <v>279</v>
+      </c>
       <c r="D122" s="54"/>
       <c r="E122" s="55" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="F122" s="54" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="G122" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H122" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="I122" s="54"/>
-      <c r="J122" s="112"/>
+        <v>137</v>
+      </c>
+      <c r="H122" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="I122" s="54">
+        <v>3.8</v>
+      </c>
+      <c r="J122" s="99"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="66" t="s">
@@ -5446,19 +5420,67 @@
       <c r="C123" s="54"/>
       <c r="D123" s="54"/>
       <c r="E123" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F123" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="G123" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="H123" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="I123" s="55">
+        <v>1436</v>
+      </c>
+      <c r="J123" s="99" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B124" s="66"/>
+      <c r="C124" s="54"/>
+      <c r="D124" s="54"/>
+      <c r="E124" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="F124" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="G124" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H124" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="I124" s="54"/>
+      <c r="J124" s="99"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B125" s="66"/>
+      <c r="C125" s="54"/>
+      <c r="D125" s="54"/>
+      <c r="E125" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="F123" s="54" t="s">
+      <c r="F125" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="G123" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H123" s="55" t="s">
+      <c r="G125" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H125" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="I123" s="54"/>
-      <c r="J123" s="112"/>
+      <c r="I125" s="54"/>
+      <c r="J125" s="99"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5467,21 +5489,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F57573F99DE79145B2C4B20841E12603" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bffb4cedf0b3900262138fdae33e2dc4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0c1e910d-4918-42f1-af2c-ed1101d63abc" xmlns:ns4="786e620f-b1da-4f59-878c-ef7546d25bf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37173867f386110bdd2a41aaff59b7e1" ns3:_="" ns4:_="">
     <xsd:import namespace="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
@@ -5710,32 +5717,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE73DB8-1736-4671-8FD3-622DFFD73211}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D01498-1E58-48D4-ACAD-5E74F94105E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5752,4 +5749,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE73DB8-1736-4671-8FD3-622DFFD73211}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Relax DWI echo time constraint for new leeds data
</commit_message>
<xml_diff>
--- a/config/ukrin_conf.xlsx
+++ b/config/ukrin_conf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\martin\code\xnat-dicomqc\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5BEB1F-BDE1-4D5E-9219-87E762A73658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEFF542-F467-417C-9543-7D73925994BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="300" windowWidth="25890" windowHeight="14745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series names" sheetId="2" r:id="rId1"/>
@@ -881,9 +881,6 @@
     <t>[4.92, 9.84]</t>
   </si>
   <si>
-    <t>[45, 65]</t>
-  </si>
-  <si>
     <t>T1MAP,T1MAP_FLIPPED,T2_MAPPING,T2STAR,BASE,FAIR,PCASL</t>
   </si>
   <si>
@@ -918,6 +915,9 @@
   </si>
   <si>
     <t>[45, 67.5]</t>
+  </si>
+  <si>
+    <t>[45, 66]</t>
   </si>
 </sst>
 </file>
@@ -2489,8 +2489,8 @@
   <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,7 +2538,7 @@
         <v>76</v>
       </c>
       <c r="J1" s="83" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>206</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B3" s="81" t="s">
         <v>221</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" s="81" t="s">
         <v>221</v>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" t="s">
@@ -2704,7 +2704,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B9" s="72"/>
       <c r="E9" s="2" t="s">
@@ -2800,7 +2800,7 @@
         <v>276</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K13" t="s">
         <v>100</v>
@@ -2808,7 +2808,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" t="s">
@@ -2832,7 +2832,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B15" s="72"/>
       <c r="C15" t="s">
@@ -4048,7 +4048,7 @@
         <v>137</v>
       </c>
       <c r="H66" s="27" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="I66" s="27">
         <v>65</v>
@@ -4074,7 +4074,7 @@
         <v>137</v>
       </c>
       <c r="H67" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I67" s="27">
         <v>65</v>
@@ -4083,7 +4083,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B68" s="58"/>
       <c r="C68" s="27" t="s">
@@ -4605,7 +4605,7 @@
         <v>137</v>
       </c>
       <c r="H89" s="38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I89" s="38">
         <v>481.8</v>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="I96" s="42"/>
       <c r="J96" s="94" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -4799,7 +4799,7 @@
         <v>63</v>
       </c>
       <c r="J97" s="94" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
         <v>739.8</v>
       </c>
       <c r="J98" s="94" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -4989,7 +4989,7 @@
         <v>137</v>
       </c>
       <c r="H105" s="47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I105" s="47"/>
       <c r="J105" s="95"/>
@@ -5435,7 +5435,7 @@
         <v>1436</v>
       </c>
       <c r="J123" s="99" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -5489,6 +5489,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F57573F99DE79145B2C4B20841E12603" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bffb4cedf0b3900262138fdae33e2dc4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0c1e910d-4918-42f1-af2c-ed1101d63abc" xmlns:ns4="786e620f-b1da-4f59-878c-ef7546d25bf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37173867f386110bdd2a41aaff59b7e1" ns3:_="" ns4:_="">
     <xsd:import namespace="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
@@ -5717,22 +5732,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE73DB8-1736-4671-8FD3-622DFFD73211}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D01498-1E58-48D4-ACAD-5E74F94105E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5749,29 +5774,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE73DB8-1736-4671-8FD3-622DFFD73211}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to fix some tests for GE scanners
</commit_message>
<xml_diff>
--- a/config/ukrin_conf.xlsx
+++ b/config/ukrin_conf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\martin\code\xnat-dicomqc\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbzmsc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEFF542-F467-417C-9543-7D73925994BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC25ADF-FCF0-4D72-9D30-5315ABFA3AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="300" windowWidth="25890" windowHeight="14745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series names" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="294">
   <si>
     <t>Vendors</t>
   </si>
@@ -503,9 +503,6 @@
     <t>[0.672, 1]</t>
   </si>
   <si>
-    <t>[800, 1000]</t>
-  </si>
-  <si>
     <t>[55, 65]</t>
   </si>
   <si>
@@ -650,9 +647,6 @@
     <t>MOLLI,T2STAR,MTR,T1W,T2W</t>
   </si>
   <si>
-    <t>[130, 170]</t>
-  </si>
-  <si>
     <t>130 is correct but don't want to fail existing data</t>
   </si>
   <si>
@@ -851,9 +845,6 @@
     <t>p2</t>
   </si>
   <si>
-    <t>p3</t>
-  </si>
-  <si>
     <t>[20, 35]</t>
   </si>
   <si>
@@ -914,10 +905,19 @@
     <t>[320, 600]</t>
   </si>
   <si>
-    <t>[45, 67.5]</t>
-  </si>
-  <si>
-    <t>[45, 66]</t>
+    <t>[3000, 10000]</t>
+  </si>
+  <si>
+    <t>[750, 1000]</t>
+  </si>
+  <si>
+    <t>[130, 180]</t>
+  </si>
+  <si>
+    <t>[45, 70]</t>
+  </si>
+  <si>
+    <t>Phillips</t>
   </si>
 </sst>
 </file>
@@ -1548,24 +1548,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1582,12 +1582,12 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1603,21 +1603,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
         <v>199</v>
-      </c>
-      <c r="B7" t="s">
-        <v>200</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C8" t="s">
         <v>51</v>
@@ -1642,32 +1642,32 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1694,13 +1694,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1730,7 +1730,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1747,7 +1747,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,7 +1758,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1802,7 +1802,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,57 +1829,57 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="79" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="79" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="77" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="79" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="79" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="78" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="80" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,7 +1890,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="80" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,35 +1906,35 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="78" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="80" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="78" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="80" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="78" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="80" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1950,13 +1950,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1964,13 +1964,13 @@
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,7 +1981,7 @@
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C44" t="s">
         <v>33</v>
@@ -2039,7 +2039,7 @@
         <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2050,7 +2050,7 @@
         <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2094,7 +2094,7 @@
         <v>33</v>
       </c>
       <c r="D50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2105,7 +2105,7 @@
         <v>33</v>
       </c>
       <c r="D51" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,27 +2116,27 @@
         <v>33</v>
       </c>
       <c r="D52" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>33</v>
       </c>
       <c r="D58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2169,7 +2169,7 @@
         <v>33</v>
       </c>
       <c r="D59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2180,7 +2180,7 @@
         <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>33</v>
       </c>
       <c r="D61" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2222,7 +2222,7 @@
         <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>51</v>
       </c>
       <c r="D65" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>51</v>
       </c>
       <c r="D66" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2266,7 +2266,7 @@
         <v>51</v>
       </c>
       <c r="D68" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,7 +2277,7 @@
         <v>51</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2288,12 +2288,12 @@
         <v>51</v>
       </c>
       <c r="D70" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C71" t="s">
         <v>51</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C73" t="s">
         <v>51</v>
@@ -2326,13 +2326,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C74" t="s">
         <v>51</v>
       </c>
       <c r="D74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
         <v>51</v>
       </c>
       <c r="D75" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
         <v>51</v>
       </c>
       <c r="D76" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
         <v>51</v>
       </c>
       <c r="D78" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2387,7 +2387,7 @@
         <v>51</v>
       </c>
       <c r="D79" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>51</v>
       </c>
       <c r="D80" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2409,18 +2409,18 @@
         <v>51</v>
       </c>
       <c r="D81" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C82" t="s">
         <v>51</v>
       </c>
       <c r="D82" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2431,7 +2431,7 @@
         <v>51</v>
       </c>
       <c r="D83" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2453,7 +2453,7 @@
         <v>51</v>
       </c>
       <c r="D85" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,7 +2464,7 @@
         <v>51</v>
       </c>
       <c r="D86" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2475,7 +2475,7 @@
         <v>51</v>
       </c>
       <c r="D87" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2486,11 +2486,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L125"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,10 +2511,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2538,15 +2538,15 @@
         <v>76</v>
       </c>
       <c r="J1" s="83" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B2" s="72"/>
       <c r="C2" t="s">
@@ -2567,10 +2567,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
         <v>81</v>
@@ -2590,10 +2590,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
         <v>83</v>
@@ -2611,13 +2611,13 @@
         <v>5</v>
       </c>
       <c r="K4" s="60" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L4" s="60"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" t="s">
@@ -2638,7 +2638,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" t="s">
@@ -2663,7 +2663,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" t="s">
@@ -2684,10 +2684,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B8" s="81" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>92</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B9" s="72"/>
       <c r="E9" s="2" t="s">
@@ -2722,7 +2722,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" s="3"/>
       <c r="E10" s="2" t="s">
@@ -2740,7 +2740,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B11" s="72"/>
       <c r="E11" s="2" t="s">
@@ -2797,10 +2797,10 @@
         <v>79</v>
       </c>
       <c r="H13" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="K13" t="s">
         <v>100</v>
@@ -2808,7 +2808,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" t="s">
@@ -2832,14 +2832,14 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B15" s="72"/>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F15" t="s">
         <v>102</v>
@@ -2848,12 +2848,12 @@
         <v>79</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" t="s">
@@ -2877,7 +2877,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" t="s">
@@ -2898,7 +2898,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B18" s="72"/>
       <c r="C18" s="82" t="s">
@@ -2919,7 +2919,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="82" t="s">
@@ -2940,7 +2940,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B20" s="72"/>
       <c r="C20" s="82" t="s">
@@ -2961,14 +2961,14 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="82" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F21" t="s">
         <v>117</v>
@@ -2982,14 +2982,14 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B22" s="72"/>
       <c r="C22" s="82" t="s">
         <v>51</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F22" t="s">
         <v>117</v>
@@ -3006,7 +3006,7 @@
         <v>118</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="69"/>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="6" t="s">
@@ -3051,7 +3051,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="6" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="11" t="s">
@@ -3099,7 +3099,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="6" t="s">
@@ -3116,14 +3116,14 @@
         <v>128</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="85"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="6"/>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="6"/>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="6"/>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="12" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="15" t="s">
@@ -3326,7 +3326,7 @@
         <v>137</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>141</v>
+        <v>289</v>
       </c>
       <c r="I36" s="12"/>
       <c r="J36" s="86"/>
@@ -3413,7 +3413,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>102</v>
@@ -3422,7 +3422,7 @@
         <v>79</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I40" s="12"/>
       <c r="J40" s="86"/>
@@ -3753,7 +3753,7 @@
         <v>137</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>155</v>
+        <v>290</v>
       </c>
       <c r="I54" s="22">
         <v>877</v>
@@ -3851,7 +3851,7 @@
         <v>137</v>
       </c>
       <c r="H58" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I58" s="22">
         <v>62</v>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B63" s="58"/>
       <c r="C63" s="26"/>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B64" s="58"/>
       <c r="C64" s="27" t="s">
@@ -4007,7 +4007,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B65" s="58"/>
       <c r="C65" s="27"/>
@@ -4022,7 +4022,7 @@
         <v>137</v>
       </c>
       <c r="H65" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I65" s="27">
         <v>1988</v>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B66" s="58"/>
       <c r="C66" s="27" t="s">
@@ -4048,7 +4048,7 @@
         <v>137</v>
       </c>
       <c r="H66" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I66" s="27">
         <v>65</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B67" s="58"/>
       <c r="C67" s="27" t="s">
@@ -4083,7 +4083,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="58" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B68" s="58"/>
       <c r="C68" s="27" t="s">
@@ -4107,7 +4107,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B69" s="58"/>
       <c r="C69" s="27" t="s">
@@ -4134,7 +4134,7 @@
         <v>5</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C70" s="30" t="s">
         <v>2</v>
@@ -4160,7 +4160,7 @@
         <v>5</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C71" s="30" t="s">
         <v>149</v>
@@ -4176,7 +4176,7 @@
         <v>128</v>
       </c>
       <c r="H71" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I71" s="30"/>
       <c r="J71" s="91"/>
@@ -4186,7 +4186,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C72" s="30" t="s">
         <v>33</v>
@@ -4202,7 +4202,7 @@
         <v>128</v>
       </c>
       <c r="H72" s="30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I72" s="30"/>
       <c r="J72" s="30"/>
@@ -4212,7 +4212,7 @@
         <v>5</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C73" s="30"/>
       <c r="D73" s="30"/>
@@ -4223,10 +4223,10 @@
         <v>131</v>
       </c>
       <c r="G73" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I73" s="30"/>
       <c r="J73" s="30"/>
@@ -4236,7 +4236,7 @@
         <v>5</v>
       </c>
       <c r="B74" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C74" s="30"/>
       <c r="D74" s="30"/>
@@ -4247,15 +4247,15 @@
         <v>134</v>
       </c>
       <c r="G74" s="30" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="H74" s="30" t="s">
-        <v>204</v>
+        <v>291</v>
       </c>
       <c r="I74" s="30"/>
       <c r="J74" s="30"/>
       <c r="K74" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -4263,7 +4263,7 @@
         <v>5</v>
       </c>
       <c r="B75" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C75" s="30"/>
       <c r="D75" s="30"/>
@@ -4301,7 +4301,7 @@
         <v>137</v>
       </c>
       <c r="H76" s="35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I76" s="34">
         <v>1.68</v>
@@ -4325,7 +4325,7 @@
         <v>79</v>
       </c>
       <c r="H77" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I77" s="34"/>
       <c r="J77" s="92"/>
@@ -4347,7 +4347,7 @@
         <v>137</v>
       </c>
       <c r="H78" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I78" s="34">
         <v>3.4</v>
@@ -4388,10 +4388,10 @@
       </c>
       <c r="D80" s="34"/>
       <c r="E80" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F80" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="F80" s="34" t="s">
-        <v>163</v>
       </c>
       <c r="G80" s="36"/>
       <c r="H80" s="35"/>
@@ -4406,10 +4406,10 @@
       <c r="C81" s="34"/>
       <c r="D81" s="34"/>
       <c r="E81" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="F81" s="34" t="s">
         <v>164</v>
-      </c>
-      <c r="F81" s="34" t="s">
-        <v>165</v>
       </c>
       <c r="G81" s="36" t="s">
         <v>79</v>
@@ -4430,10 +4430,10 @@
       </c>
       <c r="D82" s="34"/>
       <c r="E82" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="F82" s="34" t="s">
         <v>166</v>
-      </c>
-      <c r="F82" s="34" t="s">
-        <v>167</v>
       </c>
       <c r="G82" s="36" t="s">
         <v>79</v>
@@ -4449,150 +4449,152 @@
         <v>9</v>
       </c>
       <c r="B83" s="63"/>
-      <c r="C83" s="34"/>
+      <c r="C83" s="34" t="s">
+        <v>293</v>
+      </c>
       <c r="D83" s="34"/>
       <c r="E83" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F83" s="34" t="s">
         <v>168</v>
-      </c>
-      <c r="F83" s="34" t="s">
-        <v>169</v>
       </c>
       <c r="G83" s="36" t="s">
         <v>128</v>
       </c>
       <c r="H83" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I83" s="34"/>
-      <c r="J83" s="92"/>
+      <c r="J83" s="92" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="63" t="s">
         <v>9</v>
       </c>
       <c r="B84" s="63"/>
-      <c r="C84" s="34"/>
+      <c r="C84" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="D84" s="34"/>
-      <c r="E84" s="36" t="s">
-        <v>170</v>
+      <c r="E84" s="37" t="s">
+        <v>167</v>
       </c>
       <c r="F84" s="34" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G84" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H84" s="35">
-        <v>8</v>
+        <v>128</v>
+      </c>
+      <c r="H84" s="35" t="s">
+        <v>200</v>
       </c>
       <c r="I84" s="34"/>
       <c r="J84" s="92"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="64" t="s">
-        <v>209</v>
-      </c>
-      <c r="B85" s="64"/>
-      <c r="C85" s="38"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="F85" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="G85" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="H85" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="I85" s="38">
-        <v>3.3</v>
-      </c>
-      <c r="J85" s="93"/>
+      <c r="A85" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="63"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="F85" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="G85" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="H85" s="35">
+        <v>8</v>
+      </c>
+      <c r="I85" s="34"/>
+      <c r="J85" s="92"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B86" s="64"/>
       <c r="C86" s="38"/>
       <c r="D86" s="38"/>
       <c r="E86" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F86" s="38" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G86" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H86" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="H86" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="I86" s="38"/>
+      <c r="I86" s="38">
+        <v>3.3</v>
+      </c>
       <c r="J86" s="93"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B87" s="64"/>
-      <c r="C87" s="38" t="s">
-        <v>279</v>
-      </c>
+      <c r="C87" s="38"/>
       <c r="D87" s="38"/>
       <c r="E87" s="39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F87" s="38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G87" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="H87" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="I87" s="38">
-        <v>5.5</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H87" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="I87" s="38"/>
       <c r="J87" s="93"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B88" s="64"/>
       <c r="C88" s="38" t="s">
-        <v>107</v>
+        <v>276</v>
       </c>
       <c r="D88" s="38"/>
       <c r="E88" s="39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F88" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="G88" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G88" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="H88" s="38" t="s">
-        <v>275</v>
+      <c r="H88" s="41" t="s">
+        <v>171</v>
       </c>
       <c r="I88" s="38">
-        <v>481.8</v>
+        <v>5.5</v>
       </c>
       <c r="J88" s="93"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B89" s="64"/>
       <c r="C89" s="38" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D89" s="38"/>
       <c r="E89" s="39" t="s">
@@ -4605,7 +4607,7 @@
         <v>137</v>
       </c>
       <c r="H89" s="38" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="I89" s="38">
         <v>481.8</v>
@@ -4614,57 +4616,59 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B90" s="64"/>
-      <c r="C90" s="38"/>
+      <c r="C90" s="38" t="s">
+        <v>51</v>
+      </c>
       <c r="D90" s="38"/>
       <c r="E90" s="39" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="F90" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="G90" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H90" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="I90" s="38"/>
+        <v>136</v>
+      </c>
+      <c r="G90" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="H90" s="38" t="s">
+        <v>288</v>
+      </c>
+      <c r="I90" s="38">
+        <v>481.8</v>
+      </c>
       <c r="J90" s="93"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B91" s="64"/>
-      <c r="C91" s="38" t="s">
-        <v>107</v>
-      </c>
+      <c r="C91" s="38"/>
       <c r="D91" s="38"/>
       <c r="E91" s="39" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="F91" s="38" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G91" s="40" t="s">
         <v>79</v>
       </c>
       <c r="H91" s="39" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="I91" s="38"/>
       <c r="J91" s="93"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B92" s="64"/>
       <c r="C92" s="38" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D92" s="38"/>
       <c r="E92" s="39" t="s">
@@ -4677,77 +4681,79 @@
         <v>79</v>
       </c>
       <c r="H92" s="39" t="s">
-        <v>174</v>
+        <v>98</v>
       </c>
       <c r="I92" s="38"/>
       <c r="J92" s="93"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B93" s="64"/>
       <c r="C93" s="38" t="s">
-        <v>175</v>
+        <v>51</v>
       </c>
       <c r="D93" s="38"/>
-      <c r="E93" s="40" t="s">
-        <v>176</v>
+      <c r="E93" s="39" t="s">
+        <v>95</v>
       </c>
       <c r="F93" s="38" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
       <c r="G93" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="H93" s="41">
-        <v>40</v>
+      <c r="H93" s="39" t="s">
+        <v>173</v>
       </c>
       <c r="I93" s="38"/>
       <c r="J93" s="93"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B94" s="67"/>
-      <c r="C94" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D94" s="42"/>
-      <c r="E94" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="F94" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="G94" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H94" s="45">
-        <v>1</v>
-      </c>
-      <c r="I94" s="42"/>
-      <c r="J94" s="94"/>
+      <c r="A94" s="64" t="s">
+        <v>207</v>
+      </c>
+      <c r="B94" s="64"/>
+      <c r="C94" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="D94" s="38"/>
+      <c r="E94" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F94" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="G94" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H94" s="41">
+        <v>40</v>
+      </c>
+      <c r="I94" s="38"/>
+      <c r="J94" s="93"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B95" s="67"/>
-      <c r="C95" s="42"/>
+      <c r="C95" s="42" t="s">
+        <v>2</v>
+      </c>
       <c r="D95" s="42"/>
       <c r="E95" s="43" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="F95" s="42" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="G95" s="44" t="s">
         <v>79</v>
       </c>
       <c r="H95" s="45">
-        <v>4.5999999999999996</v>
+        <v>1</v>
       </c>
       <c r="I95" s="42"/>
       <c r="J95" s="94"/>
@@ -4760,46 +4766,42 @@
       <c r="C96" s="42"/>
       <c r="D96" s="42"/>
       <c r="E96" s="43" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F96" s="42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G96" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H96" s="43" t="s">
-        <v>178</v>
+      <c r="H96" s="45">
+        <v>4.5999999999999996</v>
       </c>
       <c r="I96" s="42"/>
-      <c r="J96" s="94" t="s">
-        <v>287</v>
-      </c>
+      <c r="J96" s="94"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B97" s="67"/>
-      <c r="C97" s="43"/>
-      <c r="D97" s="43"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
       <c r="E97" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="F97" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="G97" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="H97" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="I97" s="42">
-        <v>63</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F97" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="G97" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H97" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="I97" s="42"/>
       <c r="J97" s="94" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
@@ -4810,22 +4812,22 @@
       <c r="C98" s="43"/>
       <c r="D98" s="43"/>
       <c r="E98" s="43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F98" s="43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G98" s="43" t="s">
         <v>137</v>
       </c>
       <c r="H98" s="45" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="I98" s="42">
-        <v>739.8</v>
+        <v>63</v>
       </c>
       <c r="J98" s="94" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -4833,24 +4835,26 @@
         <v>26</v>
       </c>
       <c r="B99" s="67"/>
-      <c r="C99" s="43" t="s">
-        <v>2</v>
-      </c>
+      <c r="C99" s="43"/>
       <c r="D99" s="43"/>
       <c r="E99" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="F99" s="42" t="s">
-        <v>102</v>
+        <v>135</v>
+      </c>
+      <c r="F99" s="43" t="s">
+        <v>136</v>
       </c>
       <c r="G99" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="H99" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="I99" s="42"/>
-      <c r="J99" s="94"/>
+        <v>137</v>
+      </c>
+      <c r="H99" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="I99" s="42">
+        <v>739.8</v>
+      </c>
+      <c r="J99" s="94" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="67" t="s">
@@ -4858,20 +4862,20 @@
       </c>
       <c r="B100" s="67"/>
       <c r="C100" s="43" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="D100" s="43"/>
       <c r="E100" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F100" s="43" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="F100" s="42" t="s">
+        <v>102</v>
       </c>
       <c r="G100" s="43" t="s">
         <v>79</v>
       </c>
       <c r="H100" s="43" t="s">
-        <v>180</v>
+        <v>103</v>
       </c>
       <c r="I100" s="42"/>
       <c r="J100" s="94"/>
@@ -4881,21 +4885,21 @@
         <v>26</v>
       </c>
       <c r="B101" s="67"/>
-      <c r="C101" s="42" t="s">
+      <c r="C101" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D101" s="42"/>
-      <c r="E101" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="F101" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="G101" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H101" s="45">
-        <v>1</v>
+      <c r="D101" s="43"/>
+      <c r="E101" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F101" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G101" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="H101" s="43" t="s">
+        <v>179</v>
       </c>
       <c r="I101" s="42"/>
       <c r="J101" s="94"/>
@@ -4906,395 +4910,395 @@
       </c>
       <c r="B102" s="67"/>
       <c r="C102" s="42" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D102" s="42"/>
-      <c r="E102" s="43" t="s">
-        <v>182</v>
+      <c r="E102" s="44" t="s">
+        <v>180</v>
       </c>
       <c r="F102" s="42" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="G102" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H102" s="45" t="s">
-        <v>184</v>
+      <c r="H102" s="45">
+        <v>1</v>
       </c>
       <c r="I102" s="42"/>
       <c r="J102" s="94"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="46" t="s">
-        <v>222</v>
-      </c>
-      <c r="B103" s="46"/>
-      <c r="C103" s="47" t="s">
+      <c r="A103" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="67"/>
+      <c r="C103" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D103" s="47"/>
-      <c r="E103" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="F103" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G103" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="H103" s="47">
-        <v>31</v>
-      </c>
-      <c r="I103" s="47"/>
-      <c r="J103" s="47"/>
+      <c r="D103" s="42"/>
+      <c r="E103" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="F103" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="G103" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H103" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="I103" s="42"/>
+      <c r="J103" s="94"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B104" s="46"/>
       <c r="C104" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D104" s="47"/>
-      <c r="E104" s="48" t="s">
-        <v>122</v>
+      <c r="E104" s="47" t="s">
+        <v>88</v>
       </c>
       <c r="F104" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="G104" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="H104" s="50" t="s">
-        <v>186</v>
+        <v>89</v>
+      </c>
+      <c r="G104" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="H104" s="47">
+        <v>31</v>
       </c>
       <c r="I104" s="47"/>
-      <c r="J104" s="95"/>
+      <c r="J104" s="47"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B105" s="46"/>
-      <c r="C105" s="47"/>
+      <c r="C105" s="47" t="s">
+        <v>2</v>
+      </c>
       <c r="D105" s="47"/>
       <c r="E105" s="48" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F105" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="G105" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="H105" s="47" t="s">
-        <v>290</v>
+        <v>123</v>
+      </c>
+      <c r="G105" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="H105" s="50" t="s">
+        <v>185</v>
       </c>
       <c r="I105" s="47"/>
       <c r="J105" s="95"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B106" s="46"/>
       <c r="C106" s="47"/>
       <c r="D106" s="47"/>
       <c r="E106" s="48" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F106" s="47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G106" s="47" t="s">
         <v>137</v>
       </c>
       <c r="H106" s="47" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="I106" s="47"/>
       <c r="J106" s="95"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B107" s="46"/>
       <c r="C107" s="47"/>
       <c r="D107" s="47"/>
       <c r="E107" s="48" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F107" s="47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G107" s="47" t="s">
         <v>137</v>
       </c>
       <c r="H107" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="I107" s="47">
+        <v>266</v>
+      </c>
+      <c r="I107" s="47"/>
+      <c r="J107" s="95"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B108" s="46"/>
+      <c r="C108" s="47"/>
+      <c r="D108" s="47"/>
+      <c r="E108" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F108" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G108" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H108" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="I108" s="47">
         <v>2034</v>
       </c>
-      <c r="J107" s="95"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="65" t="s">
-        <v>236</v>
-      </c>
-      <c r="B108" s="65" t="s">
-        <v>221</v>
-      </c>
-      <c r="C108" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D108" s="51"/>
-      <c r="E108" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="F108" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="G108" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="H108" s="52" t="s">
-        <v>187</v>
-      </c>
-      <c r="I108" s="51"/>
-      <c r="J108" s="96"/>
+      <c r="J108" s="95"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="65" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B109" s="65" t="s">
-        <v>221</v>
-      </c>
-      <c r="C109" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="D109" s="74"/>
-      <c r="E109" s="75" t="s">
-        <v>91</v>
-      </c>
-      <c r="F109" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="C109" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" s="51"/>
+      <c r="E109" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F109" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="G109" s="75" t="s">
-        <v>79</v>
-      </c>
-      <c r="H109" s="76">
-        <v>5</v>
-      </c>
-      <c r="I109" s="74"/>
-      <c r="J109" s="97"/>
+      <c r="G109" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="H109" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="I109" s="51"/>
+      <c r="J109" s="96"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="65" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B110" s="65" t="s">
-        <v>221</v>
-      </c>
-      <c r="C110" s="51"/>
-      <c r="D110" s="51"/>
-      <c r="E110" s="52" t="s">
-        <v>130</v>
-      </c>
-      <c r="F110" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="G110" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="H110" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="I110" s="51"/>
-      <c r="J110" s="96"/>
+        <v>219</v>
+      </c>
+      <c r="C110" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D110" s="74"/>
+      <c r="E110" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="F110" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="G110" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="H110" s="76">
+        <v>5</v>
+      </c>
+      <c r="I110" s="74"/>
+      <c r="J110" s="97"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="65" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B111" s="65" t="s">
-        <v>221</v>
-      </c>
-      <c r="C111" s="51" t="s">
-        <v>107</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C111" s="51"/>
       <c r="D111" s="51"/>
-      <c r="E111" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="F111" s="53" t="s">
-        <v>134</v>
+      <c r="E111" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F111" s="51" t="s">
+        <v>131</v>
       </c>
       <c r="G111" s="53" t="s">
-        <v>137</v>
-      </c>
-      <c r="H111" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="I111" s="53">
-        <v>3000</v>
-      </c>
-      <c r="J111" s="98"/>
+        <v>79</v>
+      </c>
+      <c r="H111" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="I111" s="51"/>
+      <c r="J111" s="96"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="65" t="s">
-        <v>237</v>
-      </c>
-      <c r="B112" s="65"/>
+        <v>234</v>
+      </c>
+      <c r="B112" s="65" t="s">
+        <v>219</v>
+      </c>
       <c r="C112" s="51" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D112" s="51"/>
-      <c r="E112" s="51" t="s">
+      <c r="E112" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="F112" s="51" t="s">
+      <c r="F112" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="G112" s="51" t="s">
+      <c r="G112" s="53" t="s">
         <v>137</v>
       </c>
       <c r="H112" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="I112" s="51">
-        <v>6000</v>
-      </c>
-      <c r="J112" s="51"/>
+        <v>289</v>
+      </c>
+      <c r="I112" s="53">
+        <v>3000</v>
+      </c>
+      <c r="J112" s="98"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="65" t="s">
-        <v>236</v>
-      </c>
-      <c r="B113" s="65" t="s">
-        <v>221</v>
-      </c>
-      <c r="C113" s="51"/>
+        <v>235</v>
+      </c>
+      <c r="B113" s="65"/>
+      <c r="C113" s="51" t="s">
+        <v>51</v>
+      </c>
       <c r="D113" s="51"/>
       <c r="E113" s="51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F113" s="51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G113" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="H113" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="I113" s="51" t="s">
-        <v>188</v>
+      <c r="H113" s="53" t="s">
+        <v>289</v>
+      </c>
+      <c r="I113" s="51">
+        <v>6000</v>
       </c>
       <c r="J113" s="51"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="65" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B114" s="65" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C114" s="51"/>
       <c r="D114" s="51"/>
       <c r="E114" s="51" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F114" s="51" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="G114" s="51" t="s">
         <v>137</v>
       </c>
       <c r="H114" s="51" t="s">
-        <v>272</v>
+        <v>156</v>
       </c>
       <c r="I114" s="51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J114" s="51"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="65" t="s">
-        <v>211</v>
-      </c>
-      <c r="B115" s="65"/>
+        <v>234</v>
+      </c>
+      <c r="B115" s="65" t="s">
+        <v>219</v>
+      </c>
       <c r="C115" s="51"/>
       <c r="D115" s="51"/>
       <c r="E115" s="51" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F115" s="51" t="s">
-        <v>190</v>
+        <v>127</v>
       </c>
       <c r="G115" s="51" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="H115" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="I115" s="51"/>
+        <v>269</v>
+      </c>
+      <c r="I115" s="51" t="s">
+        <v>188</v>
+      </c>
       <c r="J115" s="51"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="65" t="s">
-        <v>210</v>
-      </c>
-      <c r="B116" s="65" t="s">
-        <v>234</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B116" s="65"/>
       <c r="C116" s="51"/>
       <c r="D116" s="51"/>
       <c r="E116" s="51" t="s">
         <v>119</v>
       </c>
       <c r="F116" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G116" s="51" t="s">
         <v>79</v>
       </c>
       <c r="H116" s="51" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="I116" s="51"/>
       <c r="J116" s="51"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="B117" s="65"/>
-      <c r="C117" s="51" t="s">
-        <v>2</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B117" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="C117" s="51"/>
       <c r="D117" s="51"/>
       <c r="E117" s="51" t="s">
         <v>119</v>
       </c>
       <c r="F117" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G117" s="51" t="s">
         <v>79</v>
       </c>
       <c r="H117" s="51" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="I117" s="51"/>
       <c r="J117" s="51"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="65" t="s">
-        <v>239</v>
+        <v>28</v>
       </c>
       <c r="B118" s="65"/>
       <c r="C118" s="51" t="s">
@@ -5305,20 +5309,20 @@
         <v>119</v>
       </c>
       <c r="F118" s="51" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="G118" s="51" t="s">
         <v>79</v>
       </c>
       <c r="H118" s="51" t="s">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="I118" s="51"/>
       <c r="J118" s="51"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="65" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B119" s="65"/>
       <c r="C119" s="51" t="s">
@@ -5335,34 +5339,34 @@
         <v>79</v>
       </c>
       <c r="H119" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I119" s="51"/>
       <c r="J119" s="51"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B120" s="66"/>
-      <c r="C120" s="54"/>
-      <c r="D120" s="54"/>
-      <c r="E120" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="F120" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="G120" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="H120" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="I120" s="54">
-        <v>2.5</v>
-      </c>
-      <c r="J120" s="99"/>
+      <c r="A120" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="B120" s="65"/>
+      <c r="C120" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D120" s="51"/>
+      <c r="E120" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F120" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="G120" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H120" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="I120" s="51"/>
+      <c r="J120" s="51"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="66" t="s">
@@ -5372,18 +5376,20 @@
       <c r="C121" s="54"/>
       <c r="D121" s="54"/>
       <c r="E121" s="55" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F121" s="54" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G121" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H121" s="55" t="s">
-        <v>192</v>
-      </c>
-      <c r="I121" s="54"/>
+        <v>137</v>
+      </c>
+      <c r="H121" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="I121" s="54">
+        <v>2.5</v>
+      </c>
       <c r="J121" s="99"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
@@ -5391,25 +5397,21 @@
         <v>31</v>
       </c>
       <c r="B122" s="66"/>
-      <c r="C122" s="54" t="s">
-        <v>279</v>
-      </c>
+      <c r="C122" s="54"/>
       <c r="D122" s="54"/>
       <c r="E122" s="55" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F122" s="54" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G122" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="H122" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="I122" s="54">
-        <v>3.8</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H122" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="I122" s="54"/>
       <c r="J122" s="99"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -5417,26 +5419,26 @@
         <v>31</v>
       </c>
       <c r="B123" s="66"/>
-      <c r="C123" s="54"/>
+      <c r="C123" s="54" t="s">
+        <v>276</v>
+      </c>
       <c r="D123" s="54"/>
       <c r="E123" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="F123" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="G123" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F123" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="G123" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="H123" s="55" t="s">
-        <v>274</v>
-      </c>
-      <c r="I123" s="55">
-        <v>1436</v>
-      </c>
-      <c r="J123" s="99" t="s">
-        <v>287</v>
-      </c>
+      <c r="H123" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="I123" s="54">
+        <v>3.8</v>
+      </c>
+      <c r="J123" s="99"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="66" t="s">
@@ -5446,19 +5448,23 @@
       <c r="C124" s="54"/>
       <c r="D124" s="54"/>
       <c r="E124" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="F124" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="G124" s="56" t="s">
-        <v>79</v>
+        <v>135</v>
+      </c>
+      <c r="F124" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="G124" s="55" t="s">
+        <v>137</v>
       </c>
       <c r="H124" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="I124" s="54"/>
-      <c r="J124" s="99"/>
+        <v>271</v>
+      </c>
+      <c r="I124" s="55">
+        <v>1436</v>
+      </c>
+      <c r="J124" s="99" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="66" t="s">
@@ -5468,19 +5474,41 @@
       <c r="C125" s="54"/>
       <c r="D125" s="54"/>
       <c r="E125" s="55" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F125" s="54" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G125" s="56" t="s">
         <v>79</v>
       </c>
       <c r="H125" s="55" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="I125" s="54"/>
       <c r="J125" s="99"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B126" s="66"/>
+      <c r="C126" s="54"/>
+      <c r="D126" s="54"/>
+      <c r="E126" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="F126" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="G126" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H126" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="I126" s="54"/>
+      <c r="J126" s="99"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correct misspelling of philips
</commit_message>
<xml_diff>
--- a/config/ukrin_conf.xlsx
+++ b/config/ukrin_conf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbzmsc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\martin\code\xnat-dicomqc\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC25ADF-FCF0-4D72-9D30-5315ABFA3AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{39552174-C5D1-4D91-AF13-45BDAFE4FFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="296">
   <si>
     <t>Vendors</t>
   </si>
@@ -917,7 +917,13 @@
     <t>[45, 70]</t>
   </si>
   <si>
-    <t>Phillips</t>
+    <t>(0018, 0082)</t>
+  </si>
+  <si>
+    <t>[235, 315]</t>
+  </si>
+  <si>
+    <t>[215, 295]</t>
   </si>
 </sst>
 </file>
@@ -2486,11 +2492,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L126"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J80" sqref="J80"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4450,7 +4456,7 @@
       </c>
       <c r="B83" s="63"/>
       <c r="C83" s="34" t="s">
-        <v>293</v>
+        <v>2</v>
       </c>
       <c r="D83" s="34"/>
       <c r="E83" s="37" t="s">
@@ -4476,11 +4482,11 @@
       </c>
       <c r="B84" s="63"/>
       <c r="C84" s="34" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="D84" s="34"/>
       <c r="E84" s="37" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="F84" s="34" t="s">
         <v>168</v>
@@ -4489,56 +4495,60 @@
         <v>128</v>
       </c>
       <c r="H84" s="35" t="s">
-        <v>200</v>
+        <v>294</v>
       </c>
       <c r="I84" s="34"/>
-      <c r="J84" s="92"/>
+      <c r="J84" s="92" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="63" t="s">
         <v>9</v>
       </c>
       <c r="B85" s="63"/>
-      <c r="C85" s="34"/>
+      <c r="C85" s="34" t="s">
+        <v>33</v>
+      </c>
       <c r="D85" s="34"/>
-      <c r="E85" s="36" t="s">
+      <c r="E85" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="F85" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="G85" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="H85" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="I85" s="34"/>
+      <c r="J85" s="92" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86" s="63"/>
+      <c r="C86" s="34"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="F85" s="34" t="s">
+      <c r="F86" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="G85" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H85" s="35">
+      <c r="G86" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="H86" s="35">
         <v>8</v>
       </c>
-      <c r="I85" s="34"/>
-      <c r="J85" s="92"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="64" t="s">
-        <v>207</v>
-      </c>
-      <c r="B86" s="64"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="F86" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="G86" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="H86" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="I86" s="38">
-        <v>3.3</v>
-      </c>
-      <c r="J86" s="93"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="92"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
@@ -4548,18 +4558,20 @@
       <c r="C87" s="38"/>
       <c r="D87" s="38"/>
       <c r="E87" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F87" s="38" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G87" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H87" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="I87" s="38"/>
+        <v>137</v>
+      </c>
+      <c r="H87" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="I87" s="38">
+        <v>3.3</v>
+      </c>
       <c r="J87" s="93"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -4567,25 +4579,21 @@
         <v>207</v>
       </c>
       <c r="B88" s="64"/>
-      <c r="C88" s="38" t="s">
-        <v>276</v>
-      </c>
+      <c r="C88" s="38"/>
       <c r="D88" s="38"/>
       <c r="E88" s="39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F88" s="38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G88" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="H88" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="I88" s="38">
-        <v>5.5</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H88" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="I88" s="38"/>
       <c r="J88" s="93"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -4594,23 +4602,23 @@
       </c>
       <c r="B89" s="64"/>
       <c r="C89" s="38" t="s">
-        <v>107</v>
+        <v>276</v>
       </c>
       <c r="D89" s="38"/>
       <c r="E89" s="39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F89" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="G89" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G89" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="H89" s="38" t="s">
-        <v>272</v>
+      <c r="H89" s="41" t="s">
+        <v>171</v>
       </c>
       <c r="I89" s="38">
-        <v>481.8</v>
+        <v>5.5</v>
       </c>
       <c r="J89" s="93"/>
     </row>
@@ -4620,7 +4628,7 @@
       </c>
       <c r="B90" s="64"/>
       <c r="C90" s="38" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D90" s="38"/>
       <c r="E90" s="39" t="s">
@@ -4633,7 +4641,7 @@
         <v>137</v>
       </c>
       <c r="H90" s="38" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="I90" s="38">
         <v>481.8</v>
@@ -4645,21 +4653,25 @@
         <v>207</v>
       </c>
       <c r="B91" s="64"/>
-      <c r="C91" s="38"/>
+      <c r="C91" s="38" t="s">
+        <v>51</v>
+      </c>
       <c r="D91" s="38"/>
       <c r="E91" s="39" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="F91" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="G91" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H91" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="I91" s="38"/>
+        <v>136</v>
+      </c>
+      <c r="G91" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="H91" s="38" t="s">
+        <v>288</v>
+      </c>
+      <c r="I91" s="38">
+        <v>481.8</v>
+      </c>
       <c r="J91" s="93"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
@@ -4667,21 +4679,19 @@
         <v>207</v>
       </c>
       <c r="B92" s="64"/>
-      <c r="C92" s="38" t="s">
-        <v>107</v>
-      </c>
+      <c r="C92" s="38"/>
       <c r="D92" s="38"/>
       <c r="E92" s="39" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="F92" s="38" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G92" s="40" t="s">
         <v>79</v>
       </c>
       <c r="H92" s="39" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="I92" s="38"/>
       <c r="J92" s="93"/>
@@ -4692,7 +4702,7 @@
       </c>
       <c r="B93" s="64"/>
       <c r="C93" s="38" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D93" s="38"/>
       <c r="E93" s="39" t="s">
@@ -4705,7 +4715,7 @@
         <v>79</v>
       </c>
       <c r="H93" s="39" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="I93" s="38"/>
       <c r="J93" s="93"/>
@@ -4716,66 +4726,68 @@
       </c>
       <c r="B94" s="64"/>
       <c r="C94" s="38" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
       <c r="D94" s="38"/>
-      <c r="E94" s="40" t="s">
-        <v>175</v>
+      <c r="E94" s="39" t="s">
+        <v>95</v>
       </c>
       <c r="F94" s="38" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="G94" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="H94" s="41">
-        <v>40</v>
+      <c r="H94" s="39" t="s">
+        <v>173</v>
       </c>
       <c r="I94" s="38"/>
       <c r="J94" s="93"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B95" s="67"/>
-      <c r="C95" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D95" s="42"/>
-      <c r="E95" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="F95" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="G95" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H95" s="45">
-        <v>1</v>
-      </c>
-      <c r="I95" s="42"/>
-      <c r="J95" s="94"/>
+      <c r="A95" s="64" t="s">
+        <v>207</v>
+      </c>
+      <c r="B95" s="64"/>
+      <c r="C95" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="D95" s="38"/>
+      <c r="E95" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F95" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="G95" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H95" s="41">
+        <v>40</v>
+      </c>
+      <c r="I95" s="38"/>
+      <c r="J95" s="93"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B96" s="67"/>
-      <c r="C96" s="42"/>
+      <c r="C96" s="42" t="s">
+        <v>2</v>
+      </c>
       <c r="D96" s="42"/>
       <c r="E96" s="43" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="F96" s="42" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="G96" s="44" t="s">
         <v>79</v>
       </c>
       <c r="H96" s="45">
-        <v>4.5999999999999996</v>
+        <v>1</v>
       </c>
       <c r="I96" s="42"/>
       <c r="J96" s="94"/>
@@ -4788,44 +4800,40 @@
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
       <c r="E97" s="43" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F97" s="42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G97" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H97" s="43" t="s">
-        <v>177</v>
+      <c r="H97" s="45">
+        <v>4.5999999999999996</v>
       </c>
       <c r="I97" s="42"/>
-      <c r="J97" s="94" t="s">
-        <v>284</v>
-      </c>
+      <c r="J97" s="94"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B98" s="67"/>
-      <c r="C98" s="43"/>
-      <c r="D98" s="43"/>
+      <c r="C98" s="42"/>
+      <c r="D98" s="42"/>
       <c r="E98" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="F98" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="G98" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="H98" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="I98" s="42">
-        <v>63</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F98" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="G98" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H98" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="I98" s="42"/>
       <c r="J98" s="94" t="s">
         <v>284</v>
       </c>
@@ -4838,19 +4846,19 @@
       <c r="C99" s="43"/>
       <c r="D99" s="43"/>
       <c r="E99" s="43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F99" s="43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G99" s="43" t="s">
         <v>137</v>
       </c>
       <c r="H99" s="45" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="I99" s="42">
-        <v>739.8</v>
+        <v>63</v>
       </c>
       <c r="J99" s="94" t="s">
         <v>284</v>
@@ -4861,24 +4869,26 @@
         <v>26</v>
       </c>
       <c r="B100" s="67"/>
-      <c r="C100" s="43" t="s">
-        <v>2</v>
-      </c>
+      <c r="C100" s="43"/>
       <c r="D100" s="43"/>
       <c r="E100" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="F100" s="42" t="s">
-        <v>102</v>
+        <v>135</v>
+      </c>
+      <c r="F100" s="43" t="s">
+        <v>136</v>
       </c>
       <c r="G100" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="H100" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="I100" s="42"/>
-      <c r="J100" s="94"/>
+        <v>137</v>
+      </c>
+      <c r="H100" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="I100" s="42">
+        <v>739.8</v>
+      </c>
+      <c r="J100" s="94" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="67" t="s">
@@ -4886,20 +4896,20 @@
       </c>
       <c r="B101" s="67"/>
       <c r="C101" s="43" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="D101" s="43"/>
       <c r="E101" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F101" s="43" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="F101" s="42" t="s">
+        <v>102</v>
       </c>
       <c r="G101" s="43" t="s">
         <v>79</v>
       </c>
       <c r="H101" s="43" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="I101" s="42"/>
       <c r="J101" s="94"/>
@@ -4909,21 +4919,21 @@
         <v>26</v>
       </c>
       <c r="B102" s="67"/>
-      <c r="C102" s="42" t="s">
+      <c r="C102" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D102" s="42"/>
-      <c r="E102" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="F102" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="G102" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H102" s="45">
-        <v>1</v>
+      <c r="D102" s="43"/>
+      <c r="E102" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F102" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G102" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="H102" s="43" t="s">
+        <v>179</v>
       </c>
       <c r="I102" s="42"/>
       <c r="J102" s="94"/>
@@ -4934,47 +4944,47 @@
       </c>
       <c r="B103" s="67"/>
       <c r="C103" s="42" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D103" s="42"/>
-      <c r="E103" s="43" t="s">
-        <v>181</v>
+      <c r="E103" s="44" t="s">
+        <v>180</v>
       </c>
       <c r="F103" s="42" t="s">
-        <v>182</v>
+        <v>89</v>
       </c>
       <c r="G103" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H103" s="45" t="s">
-        <v>183</v>
+      <c r="H103" s="45">
+        <v>1</v>
       </c>
       <c r="I103" s="42"/>
       <c r="J103" s="94"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="B104" s="46"/>
-      <c r="C104" s="47" t="s">
+      <c r="A104" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="67"/>
+      <c r="C104" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="47"/>
-      <c r="E104" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="F104" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G104" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="H104" s="47">
-        <v>31</v>
-      </c>
-      <c r="I104" s="47"/>
-      <c r="J104" s="47"/>
+      <c r="D104" s="42"/>
+      <c r="E104" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="F104" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="G104" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H104" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="I104" s="42"/>
+      <c r="J104" s="94"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="46" t="s">
@@ -4985,39 +4995,41 @@
         <v>2</v>
       </c>
       <c r="D105" s="47"/>
-      <c r="E105" s="48" t="s">
-        <v>122</v>
+      <c r="E105" s="47" t="s">
+        <v>88</v>
       </c>
       <c r="F105" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="G105" s="49" t="s">
-        <v>184</v>
-      </c>
-      <c r="H105" s="50" t="s">
-        <v>185</v>
+        <v>89</v>
+      </c>
+      <c r="G105" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="H105" s="47">
+        <v>31</v>
       </c>
       <c r="I105" s="47"/>
-      <c r="J105" s="95"/>
+      <c r="J105" s="47"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="46" t="s">
         <v>220</v>
       </c>
       <c r="B106" s="46"/>
-      <c r="C106" s="47"/>
+      <c r="C106" s="47" t="s">
+        <v>2</v>
+      </c>
       <c r="D106" s="47"/>
       <c r="E106" s="48" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F106" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="G106" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="H106" s="47" t="s">
-        <v>287</v>
+        <v>123</v>
+      </c>
+      <c r="G106" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="H106" s="50" t="s">
+        <v>185</v>
       </c>
       <c r="I106" s="47"/>
       <c r="J106" s="95"/>
@@ -5030,16 +5042,16 @@
       <c r="C107" s="47"/>
       <c r="D107" s="47"/>
       <c r="E107" s="48" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F107" s="47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G107" s="47" t="s">
         <v>137</v>
       </c>
       <c r="H107" s="47" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="I107" s="47"/>
       <c r="J107" s="95"/>
@@ -5052,47 +5064,43 @@
       <c r="C108" s="47"/>
       <c r="D108" s="47"/>
       <c r="E108" s="48" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F108" s="47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G108" s="47" t="s">
         <v>137</v>
       </c>
       <c r="H108" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="I108" s="47"/>
+      <c r="J108" s="95"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B109" s="46"/>
+      <c r="C109" s="47"/>
+      <c r="D109" s="47"/>
+      <c r="E109" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F109" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G109" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H109" s="47" t="s">
         <v>270</v>
       </c>
-      <c r="I108" s="47">
+      <c r="I109" s="47">
         <v>2034</v>
       </c>
-      <c r="J108" s="95"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="65" t="s">
-        <v>234</v>
-      </c>
-      <c r="B109" s="65" t="s">
-        <v>219</v>
-      </c>
-      <c r="C109" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D109" s="51"/>
-      <c r="E109" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="F109" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="G109" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="H109" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="I109" s="51"/>
-      <c r="J109" s="96"/>
+      <c r="J109" s="95"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="65" t="s">
@@ -5101,24 +5109,24 @@
       <c r="B110" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="D110" s="74"/>
-      <c r="E110" s="75" t="s">
-        <v>91</v>
-      </c>
-      <c r="F110" s="74" t="s">
+      <c r="C110" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" s="51"/>
+      <c r="E110" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F110" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="G110" s="75" t="s">
-        <v>79</v>
-      </c>
-      <c r="H110" s="76">
-        <v>5</v>
-      </c>
-      <c r="I110" s="74"/>
-      <c r="J110" s="97"/>
+      <c r="G110" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="H110" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="I110" s="51"/>
+      <c r="J110" s="96"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="65" t="s">
@@ -5127,22 +5135,24 @@
       <c r="B111" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="C111" s="51"/>
-      <c r="D111" s="51"/>
-      <c r="E111" s="52" t="s">
-        <v>130</v>
-      </c>
-      <c r="F111" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="G111" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="H111" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="I111" s="51"/>
-      <c r="J111" s="96"/>
+      <c r="C111" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D111" s="74"/>
+      <c r="E111" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="F111" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="G111" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="H111" s="76">
+        <v>5</v>
+      </c>
+      <c r="I111" s="74"/>
+      <c r="J111" s="97"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="65" t="s">
@@ -5151,76 +5161,74 @@
       <c r="B112" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="C112" s="51" t="s">
-        <v>107</v>
-      </c>
+      <c r="C112" s="51"/>
       <c r="D112" s="51"/>
-      <c r="E112" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="F112" s="53" t="s">
-        <v>134</v>
+      <c r="E112" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F112" s="51" t="s">
+        <v>131</v>
       </c>
       <c r="G112" s="53" t="s">
-        <v>137</v>
-      </c>
-      <c r="H112" s="53" t="s">
-        <v>289</v>
-      </c>
-      <c r="I112" s="53">
-        <v>3000</v>
-      </c>
-      <c r="J112" s="98"/>
+        <v>79</v>
+      </c>
+      <c r="H112" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="I112" s="51"/>
+      <c r="J112" s="96"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="65" t="s">
-        <v>235</v>
-      </c>
-      <c r="B113" s="65"/>
+        <v>234</v>
+      </c>
+      <c r="B113" s="65" t="s">
+        <v>219</v>
+      </c>
       <c r="C113" s="51" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D113" s="51"/>
-      <c r="E113" s="51" t="s">
+      <c r="E113" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="F113" s="51" t="s">
+      <c r="F113" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="G113" s="51" t="s">
+      <c r="G113" s="53" t="s">
         <v>137</v>
       </c>
       <c r="H113" s="53" t="s">
         <v>289</v>
       </c>
-      <c r="I113" s="51">
-        <v>6000</v>
-      </c>
-      <c r="J113" s="51"/>
+      <c r="I113" s="53">
+        <v>3000</v>
+      </c>
+      <c r="J113" s="98"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="65" t="s">
-        <v>234</v>
-      </c>
-      <c r="B114" s="65" t="s">
-        <v>219</v>
-      </c>
-      <c r="C114" s="51"/>
+        <v>235</v>
+      </c>
+      <c r="B114" s="65"/>
+      <c r="C114" s="51" t="s">
+        <v>51</v>
+      </c>
       <c r="D114" s="51"/>
       <c r="E114" s="51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F114" s="51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G114" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="H114" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="I114" s="51" t="s">
-        <v>187</v>
+      <c r="H114" s="53" t="s">
+        <v>289</v>
+      </c>
+      <c r="I114" s="51">
+        <v>6000</v>
       </c>
       <c r="J114" s="51"/>
     </row>
@@ -5234,51 +5242,53 @@
       <c r="C115" s="51"/>
       <c r="D115" s="51"/>
       <c r="E115" s="51" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F115" s="51" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="G115" s="51" t="s">
         <v>137</v>
       </c>
       <c r="H115" s="51" t="s">
-        <v>269</v>
+        <v>156</v>
       </c>
       <c r="I115" s="51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J115" s="51"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="65" t="s">
-        <v>209</v>
-      </c>
-      <c r="B116" s="65"/>
+        <v>234</v>
+      </c>
+      <c r="B116" s="65" t="s">
+        <v>219</v>
+      </c>
       <c r="C116" s="51"/>
       <c r="D116" s="51"/>
       <c r="E116" s="51" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F116" s="51" t="s">
-        <v>189</v>
+        <v>127</v>
       </c>
       <c r="G116" s="51" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="H116" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="I116" s="51"/>
+        <v>269</v>
+      </c>
+      <c r="I116" s="51" t="s">
+        <v>188</v>
+      </c>
       <c r="J116" s="51"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="65" t="s">
-        <v>208</v>
-      </c>
-      <c r="B117" s="65" t="s">
-        <v>232</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B117" s="65"/>
       <c r="C117" s="51"/>
       <c r="D117" s="51"/>
       <c r="E117" s="51" t="s">
@@ -5291,19 +5301,19 @@
         <v>79</v>
       </c>
       <c r="H117" s="51" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="I117" s="51"/>
       <c r="J117" s="51"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="B118" s="65"/>
-      <c r="C118" s="51" t="s">
-        <v>2</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B118" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="C118" s="51"/>
       <c r="D118" s="51"/>
       <c r="E118" s="51" t="s">
         <v>119</v>
@@ -5315,14 +5325,14 @@
         <v>79</v>
       </c>
       <c r="H118" s="51" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="I118" s="51"/>
       <c r="J118" s="51"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="65" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="B119" s="65"/>
       <c r="C119" s="51" t="s">
@@ -5333,20 +5343,20 @@
         <v>119</v>
       </c>
       <c r="F119" s="51" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="G119" s="51" t="s">
         <v>79</v>
       </c>
       <c r="H119" s="51" t="s">
-        <v>192</v>
+        <v>103</v>
       </c>
       <c r="I119" s="51"/>
       <c r="J119" s="51"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="65" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B120" s="65"/>
       <c r="C120" s="51" t="s">
@@ -5363,34 +5373,34 @@
         <v>79</v>
       </c>
       <c r="H120" s="51" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I120" s="51"/>
       <c r="J120" s="51"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B121" s="66"/>
-      <c r="C121" s="54"/>
-      <c r="D121" s="54"/>
-      <c r="E121" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="F121" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="G121" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="H121" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="I121" s="54">
-        <v>2.5</v>
-      </c>
-      <c r="J121" s="99"/>
+      <c r="A121" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="B121" s="65"/>
+      <c r="C121" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" s="51"/>
+      <c r="E121" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F121" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="G121" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H121" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="I121" s="51"/>
+      <c r="J121" s="51"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="66" t="s">
@@ -5400,18 +5410,20 @@
       <c r="C122" s="54"/>
       <c r="D122" s="54"/>
       <c r="E122" s="55" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F122" s="54" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G122" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H122" s="55" t="s">
-        <v>191</v>
-      </c>
-      <c r="I122" s="54"/>
+        <v>137</v>
+      </c>
+      <c r="H122" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="I122" s="54">
+        <v>2.5</v>
+      </c>
       <c r="J122" s="99"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -5419,25 +5431,21 @@
         <v>31</v>
       </c>
       <c r="B123" s="66"/>
-      <c r="C123" s="54" t="s">
-        <v>276</v>
-      </c>
+      <c r="C123" s="54"/>
       <c r="D123" s="54"/>
       <c r="E123" s="55" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F123" s="54" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G123" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="H123" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="I123" s="54">
-        <v>3.8</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H123" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="I123" s="54"/>
       <c r="J123" s="99"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -5445,26 +5453,26 @@
         <v>31</v>
       </c>
       <c r="B124" s="66"/>
-      <c r="C124" s="54"/>
+      <c r="C124" s="54" t="s">
+        <v>276</v>
+      </c>
       <c r="D124" s="54"/>
       <c r="E124" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="F124" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="G124" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F124" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="G124" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="H124" s="55" t="s">
-        <v>271</v>
-      </c>
-      <c r="I124" s="55">
-        <v>1436</v>
-      </c>
-      <c r="J124" s="99" t="s">
-        <v>284</v>
-      </c>
+      <c r="H124" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="I124" s="54">
+        <v>3.8</v>
+      </c>
+      <c r="J124" s="99"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="66" t="s">
@@ -5474,19 +5482,23 @@
       <c r="C125" s="54"/>
       <c r="D125" s="54"/>
       <c r="E125" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="F125" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="G125" s="56" t="s">
-        <v>79</v>
+        <v>135</v>
+      </c>
+      <c r="F125" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="G125" s="55" t="s">
+        <v>137</v>
       </c>
       <c r="H125" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="I125" s="54"/>
-      <c r="J125" s="99"/>
+        <v>271</v>
+      </c>
+      <c r="I125" s="55">
+        <v>1436</v>
+      </c>
+      <c r="J125" s="99" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="66" t="s">
@@ -5496,19 +5508,41 @@
       <c r="C126" s="54"/>
       <c r="D126" s="54"/>
       <c r="E126" s="55" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F126" s="54" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G126" s="56" t="s">
         <v>79</v>
       </c>
       <c r="H126" s="55" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="I126" s="54"/>
       <c r="J126" s="99"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B127" s="66"/>
+      <c r="C127" s="54"/>
+      <c r="D127" s="54"/>
+      <c r="E127" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="F127" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="G127" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H127" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="I127" s="54"/>
+      <c r="J127" s="99"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>